<commit_message>
remove / from surveys acronym
</commit_message>
<xml_diff>
--- a/02.data/_aux/LIS datasets.xlsx
+++ b/02.data/_aux/LIS datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/acastanedaa_worldbank_org/Documents/WorldBank/DECDG/PovcalNet Team/LIS_data/02.data/_aux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E26749EB-33BC-4C52-B366-8DE6F1F88FBC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0803F14E-CC74-42E6-9115-46AEE48D91EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{DA214762-5DBE-485D-812E-A8355C7FFC9F}"/>
   </bookViews>
@@ -743,15 +743,9 @@
     <t>Estonian Social Survey (ESS) / Survey on Income and Living Conditions (SILC) (Estonia)</t>
   </si>
   <si>
-    <t>ESS-LIS/SILC-LIS</t>
-  </si>
-  <si>
     <t>Income Distribution Survey (IDS) / Survey on Income and Living Conditions (SILC) (Finland)</t>
   </si>
   <si>
-    <t>IDS-LIS/SILC-LIS</t>
-  </si>
-  <si>
     <t>Household Budget Survey (BdF) (France)</t>
   </si>
   <si>
@@ -788,9 +782,6 @@
     <t>Socio-economic Panel "Living in Luxembourg" (PSELL III) / Survey on Income and Living Conditions (SILC) (Luxembourg)</t>
   </si>
   <si>
-    <t>SEP-LIS /SILC-LIS</t>
-  </si>
-  <si>
     <t>Income Distibution Survey (Norway)</t>
   </si>
   <si>
@@ -863,9 +854,6 @@
     <t>SIHCA-LIS</t>
   </si>
   <si>
-    <t>SIH-LIS/HES-LIS</t>
-  </si>
-  <si>
     <t>Survey of Consumer Finances (SCF) (Canada)</t>
   </si>
   <si>
@@ -902,9 +890,6 @@
     <t>Household Income and Expenditure Survey (HIES) and Farm Household Income and Expenditure Survey (FHES) (South Korea)</t>
   </si>
   <si>
-    <t>HIES-LIS/FHES-LIS</t>
-  </si>
-  <si>
     <t>Won</t>
   </si>
   <si>
@@ -1131,6 +1116,21 @@
   </si>
   <si>
     <t>VHLSS-LIS</t>
+  </si>
+  <si>
+    <t>ESS-SILC-LIS</t>
+  </si>
+  <si>
+    <t>IDS-SILC-LIS</t>
+  </si>
+  <si>
+    <t>SEP-SILC-LIS</t>
+  </si>
+  <si>
+    <t>SIH-HES-LIS</t>
+  </si>
+  <si>
+    <t>HIES-FHES-LIS</t>
   </si>
 </sst>
 </file>
@@ -6233,9 +6233,9 @@
   <dimension ref="A1:M366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C246" sqref="C246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10098,7 +10098,7 @@
         <v>202</v>
       </c>
       <c r="D135" t="s">
-        <v>203</v>
+        <v>328</v>
       </c>
       <c r="E135" s="79" t="s">
         <v>70</v>
@@ -10124,7 +10124,7 @@
         <v>202</v>
       </c>
       <c r="D136" t="s">
-        <v>203</v>
+        <v>328</v>
       </c>
       <c r="E136" s="79" t="s">
         <v>70</v>
@@ -10150,7 +10150,7 @@
         <v>202</v>
       </c>
       <c r="D137" t="s">
-        <v>203</v>
+        <v>328</v>
       </c>
       <c r="E137" s="79" t="s">
         <v>70</v>
@@ -10176,7 +10176,7 @@
         <v>202</v>
       </c>
       <c r="D138" t="s">
-        <v>203</v>
+        <v>328</v>
       </c>
       <c r="E138" s="79" t="s">
         <v>70</v>
@@ -10199,10 +10199,10 @@
         <v>2004</v>
       </c>
       <c r="C139" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D139" t="s">
-        <v>205</v>
+        <v>329</v>
       </c>
       <c r="E139" s="79" t="s">
         <v>70</v>
@@ -10225,10 +10225,10 @@
         <v>2007</v>
       </c>
       <c r="C140" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D140" t="s">
-        <v>205</v>
+        <v>329</v>
       </c>
       <c r="E140" s="79" t="s">
         <v>70</v>
@@ -10251,10 +10251,10 @@
         <v>2010</v>
       </c>
       <c r="C141" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D141" t="s">
-        <v>205</v>
+        <v>329</v>
       </c>
       <c r="E141" s="79" t="s">
         <v>70</v>
@@ -10277,10 +10277,10 @@
         <v>2013</v>
       </c>
       <c r="C142" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D142" t="s">
-        <v>205</v>
+        <v>329</v>
       </c>
       <c r="E142" s="79" t="s">
         <v>70</v>
@@ -10303,10 +10303,10 @@
         <v>2016</v>
       </c>
       <c r="C143" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D143" t="s">
-        <v>205</v>
+        <v>329</v>
       </c>
       <c r="E143" s="79" t="s">
         <v>70</v>
@@ -10329,7 +10329,7 @@
         <v>2005</v>
       </c>
       <c r="C144" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D144" t="s">
         <v>122</v>
@@ -10355,7 +10355,7 @@
         <v>2010</v>
       </c>
       <c r="C145" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D145" t="s">
         <v>122</v>
@@ -10381,7 +10381,7 @@
         <v>1991</v>
       </c>
       <c r="C146" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D146" t="s">
         <v>66</v>
@@ -10407,7 +10407,7 @@
         <v>1994</v>
       </c>
       <c r="C147" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D147" t="s">
         <v>66</v>
@@ -10433,7 +10433,7 @@
         <v>1995</v>
       </c>
       <c r="C148" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D148" t="s">
         <v>66</v>
@@ -10459,7 +10459,7 @@
         <v>1998</v>
       </c>
       <c r="C149" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D149" t="s">
         <v>66</v>
@@ -10485,7 +10485,7 @@
         <v>2000</v>
       </c>
       <c r="C150" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D150" t="s">
         <v>66</v>
@@ -10511,7 +10511,7 @@
         <v>2001</v>
       </c>
       <c r="C151" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D151" t="s">
         <v>66</v>
@@ -10537,7 +10537,7 @@
         <v>2002</v>
       </c>
       <c r="C152" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D152" t="s">
         <v>66</v>
@@ -10563,7 +10563,7 @@
         <v>2003</v>
       </c>
       <c r="C153" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D153" t="s">
         <v>66</v>
@@ -10589,7 +10589,7 @@
         <v>2004</v>
       </c>
       <c r="C154" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D154" t="s">
         <v>66</v>
@@ -10615,7 +10615,7 @@
         <v>2005</v>
       </c>
       <c r="C155" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D155" t="s">
         <v>66</v>
@@ -10641,7 +10641,7 @@
         <v>2006</v>
       </c>
       <c r="C156" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D156" t="s">
         <v>66</v>
@@ -10667,7 +10667,7 @@
         <v>2007</v>
       </c>
       <c r="C157" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D157" t="s">
         <v>66</v>
@@ -10693,7 +10693,7 @@
         <v>2008</v>
       </c>
       <c r="C158" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D158" t="s">
         <v>66</v>
@@ -10719,7 +10719,7 @@
         <v>2009</v>
       </c>
       <c r="C159" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D159" t="s">
         <v>66</v>
@@ -10745,7 +10745,7 @@
         <v>2010</v>
       </c>
       <c r="C160" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D160" t="s">
         <v>66</v>
@@ -10771,7 +10771,7 @@
         <v>2011</v>
       </c>
       <c r="C161" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D161" t="s">
         <v>66</v>
@@ -10797,7 +10797,7 @@
         <v>2012</v>
       </c>
       <c r="C162" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D162" t="s">
         <v>66</v>
@@ -10823,7 +10823,7 @@
         <v>2013</v>
       </c>
       <c r="C163" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D163" t="s">
         <v>66</v>
@@ -10849,7 +10849,7 @@
         <v>2014</v>
       </c>
       <c r="C164" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D164" t="s">
         <v>66</v>
@@ -10875,7 +10875,7 @@
         <v>2015</v>
       </c>
       <c r="C165" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D165" t="s">
         <v>66</v>
@@ -10901,7 +10901,7 @@
         <v>2016</v>
       </c>
       <c r="C166" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D166" t="s">
         <v>66</v>
@@ -10927,7 +10927,7 @@
         <v>2004</v>
       </c>
       <c r="C167" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D167" t="s">
         <v>197</v>
@@ -10953,7 +10953,7 @@
         <v>2007</v>
       </c>
       <c r="C168" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D168" t="s">
         <v>197</v>
@@ -10979,7 +10979,7 @@
         <v>2010</v>
       </c>
       <c r="C169" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D169" t="s">
         <v>197</v>
@@ -11005,7 +11005,7 @@
         <v>2013</v>
       </c>
       <c r="C170" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D170" t="s">
         <v>197</v>
@@ -11031,7 +11031,7 @@
         <v>2005</v>
       </c>
       <c r="C171" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D171" t="s">
         <v>167</v>
@@ -11057,7 +11057,7 @@
         <v>2007</v>
       </c>
       <c r="C172" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D172" t="s">
         <v>167</v>
@@ -11083,7 +11083,7 @@
         <v>2009</v>
       </c>
       <c r="C173" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D173" t="s">
         <v>167</v>
@@ -11109,7 +11109,7 @@
         <v>2012</v>
       </c>
       <c r="C174" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D174" t="s">
         <v>167</v>
@@ -11135,7 +11135,7 @@
         <v>2015</v>
       </c>
       <c r="C175" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D175" t="s">
         <v>167</v>
@@ -11155,13 +11155,13 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B176">
         <v>2004</v>
       </c>
       <c r="C176" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D176" t="s">
         <v>197</v>
@@ -11173,7 +11173,7 @@
         <v>2928</v>
       </c>
       <c r="G176" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I176" t="s">
         <v>194</v>
@@ -11181,13 +11181,13 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B177">
         <v>2007</v>
       </c>
       <c r="C177" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D177" t="s">
         <v>197</v>
@@ -11199,7 +11199,7 @@
         <v>2887</v>
       </c>
       <c r="G177" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I177" t="s">
         <v>194</v>
@@ -11207,13 +11207,13 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B178">
         <v>2010</v>
       </c>
       <c r="C178" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D178" t="s">
         <v>197</v>
@@ -11225,7 +11225,7 @@
         <v>3018</v>
       </c>
       <c r="G178" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I178" t="s">
         <v>194</v>
@@ -11239,7 +11239,7 @@
         <v>2004</v>
       </c>
       <c r="C179" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D179" t="s">
         <v>197</v>
@@ -11265,7 +11265,7 @@
         <v>2007</v>
       </c>
       <c r="C180" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D180" t="s">
         <v>197</v>
@@ -11291,7 +11291,7 @@
         <v>2012</v>
       </c>
       <c r="C181" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D181" t="s">
         <v>197</v>
@@ -11317,7 +11317,7 @@
         <v>2004</v>
       </c>
       <c r="C182" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D182" t="s">
         <v>108</v>
@@ -11343,7 +11343,7 @@
         <v>2008</v>
       </c>
       <c r="C183" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D183" t="s">
         <v>108</v>
@@ -11369,7 +11369,7 @@
         <v>2010</v>
       </c>
       <c r="C184" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D184" t="s">
         <v>108</v>
@@ -11395,7 +11395,7 @@
         <v>2014</v>
       </c>
       <c r="C185" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D185" t="s">
         <v>108</v>
@@ -11415,13 +11415,13 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B186">
         <v>2010</v>
       </c>
       <c r="C186" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D186" t="s">
         <v>197</v>
@@ -11441,13 +11441,13 @@
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B187">
         <v>2013</v>
       </c>
       <c r="C187" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D187" t="s">
         <v>197</v>
@@ -11473,10 +11473,10 @@
         <v>2004</v>
       </c>
       <c r="C188" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D188" t="s">
-        <v>218</v>
+        <v>330</v>
       </c>
       <c r="E188" s="79" t="s">
         <v>70</v>
@@ -11499,10 +11499,10 @@
         <v>2007</v>
       </c>
       <c r="C189" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D189" t="s">
-        <v>218</v>
+        <v>330</v>
       </c>
       <c r="E189" s="79" t="s">
         <v>70</v>
@@ -11525,10 +11525,10 @@
         <v>2010</v>
       </c>
       <c r="C190" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D190" t="s">
-        <v>218</v>
+        <v>330</v>
       </c>
       <c r="E190" s="79" t="s">
         <v>70</v>
@@ -11551,10 +11551,10 @@
         <v>2013</v>
       </c>
       <c r="C191" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D191" t="s">
-        <v>218</v>
+        <v>330</v>
       </c>
       <c r="E191" s="79" t="s">
         <v>70</v>
@@ -11577,7 +11577,7 @@
         <v>2004</v>
       </c>
       <c r="C192" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D192" t="s">
         <v>86</v>
@@ -11603,7 +11603,7 @@
         <v>2007</v>
       </c>
       <c r="C193" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D193" t="s">
         <v>169</v>
@@ -11629,7 +11629,7 @@
         <v>2010</v>
       </c>
       <c r="C194" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D194" t="s">
         <v>169</v>
@@ -11655,7 +11655,7 @@
         <v>2013</v>
       </c>
       <c r="C195" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D195" t="s">
         <v>169</v>
@@ -11681,7 +11681,7 @@
         <v>2004</v>
       </c>
       <c r="C196" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D196" t="s">
         <v>122</v>
@@ -11707,7 +11707,7 @@
         <v>2007</v>
       </c>
       <c r="C197" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D197" t="s">
         <v>122</v>
@@ -11733,7 +11733,7 @@
         <v>2010</v>
       </c>
       <c r="C198" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D198" t="s">
         <v>122</v>
@@ -11759,7 +11759,7 @@
         <v>2013</v>
       </c>
       <c r="C199" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D199" t="s">
         <v>122</v>
@@ -11785,7 +11785,7 @@
         <v>2016</v>
       </c>
       <c r="C200" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D200" t="s">
         <v>122</v>
@@ -11805,13 +11805,13 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B201">
         <v>2006</v>
       </c>
       <c r="C201" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D201" t="s">
         <v>122</v>
@@ -11823,7 +11823,7 @@
         <v>4560</v>
       </c>
       <c r="G201" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I201" t="s">
         <v>194</v>
@@ -11831,13 +11831,13 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B202">
         <v>2010</v>
       </c>
       <c r="C202" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D202" t="s">
         <v>122</v>
@@ -11849,7 +11849,7 @@
         <v>4585</v>
       </c>
       <c r="G202" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I202" t="s">
         <v>194</v>
@@ -11857,13 +11857,13 @@
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B203">
         <v>2013</v>
       </c>
       <c r="C203" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D203" t="s">
         <v>122</v>
@@ -11875,7 +11875,7 @@
         <v>4517</v>
       </c>
       <c r="G203" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I203" t="s">
         <v>194</v>
@@ -11883,13 +11883,13 @@
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B204">
         <v>2016</v>
       </c>
       <c r="C204" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D204" t="s">
         <v>122</v>
@@ -11901,7 +11901,7 @@
         <v>6457</v>
       </c>
       <c r="G204" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I204" t="s">
         <v>194</v>
@@ -11909,13 +11909,13 @@
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B205">
         <v>2004</v>
       </c>
       <c r="C205" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D205" t="s">
         <v>197</v>
@@ -11935,13 +11935,13 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B206">
         <v>2007</v>
       </c>
       <c r="C206" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D206" t="s">
         <v>197</v>
@@ -11961,13 +11961,13 @@
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B207">
         <v>2010</v>
       </c>
       <c r="C207" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D207" t="s">
         <v>197</v>
@@ -11987,13 +11987,13 @@
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B208">
         <v>2013</v>
       </c>
       <c r="C208" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D208" t="s">
         <v>197</v>
@@ -12019,7 +12019,7 @@
         <v>2004</v>
       </c>
       <c r="C209" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D209" t="s">
         <v>122</v>
@@ -12031,7 +12031,7 @@
         <v>3725</v>
       </c>
       <c r="G209" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I209" t="s">
         <v>194</v>
@@ -12045,7 +12045,7 @@
         <v>2007</v>
       </c>
       <c r="C210" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D210" t="s">
         <v>122</v>
@@ -12057,7 +12057,7 @@
         <v>3697</v>
       </c>
       <c r="G210" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I210" t="s">
         <v>194</v>
@@ -12071,7 +12071,7 @@
         <v>2010</v>
       </c>
       <c r="C211" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D211" t="s">
         <v>122</v>
@@ -12083,7 +12083,7 @@
         <v>3924</v>
       </c>
       <c r="G211" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I211" t="s">
         <v>194</v>
@@ -12097,7 +12097,7 @@
         <v>2012</v>
       </c>
       <c r="C212" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D212" t="s">
         <v>122</v>
@@ -12123,7 +12123,7 @@
         <v>2015</v>
       </c>
       <c r="C213" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D213" t="s">
         <v>122</v>
@@ -12149,7 +12149,7 @@
         <v>2004</v>
       </c>
       <c r="C214" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D214" t="s">
         <v>197</v>
@@ -12175,7 +12175,7 @@
         <v>2007</v>
       </c>
       <c r="C215" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D215" t="s">
         <v>197</v>
@@ -12201,7 +12201,7 @@
         <v>2010</v>
       </c>
       <c r="C216" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D216" t="s">
         <v>197</v>
@@ -12227,7 +12227,7 @@
         <v>2013</v>
       </c>
       <c r="C217" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D217" t="s">
         <v>197</v>
@@ -12253,7 +12253,7 @@
         <v>2016</v>
       </c>
       <c r="C218" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D218" t="s">
         <v>197</v>
@@ -12279,7 +12279,7 @@
         <v>2005</v>
       </c>
       <c r="C219" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D219" t="s">
         <v>169</v>
@@ -12305,7 +12305,7 @@
         <v>2004</v>
       </c>
       <c r="C220" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D220" t="s">
         <v>171</v>
@@ -12331,7 +12331,7 @@
         <v>2007</v>
       </c>
       <c r="C221" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D221" t="s">
         <v>197</v>
@@ -12357,7 +12357,7 @@
         <v>2010</v>
       </c>
       <c r="C222" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D222" t="s">
         <v>197</v>
@@ -12383,7 +12383,7 @@
         <v>2013</v>
       </c>
       <c r="C223" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D223" t="s">
         <v>197</v>
@@ -12409,7 +12409,7 @@
         <v>2004</v>
       </c>
       <c r="C224" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D224" t="s">
         <v>151</v>
@@ -12435,7 +12435,7 @@
         <v>2007</v>
       </c>
       <c r="C225" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D225" t="s">
         <v>151</v>
@@ -12461,7 +12461,7 @@
         <v>2010</v>
       </c>
       <c r="C226" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D226" t="s">
         <v>151</v>
@@ -12487,7 +12487,7 @@
         <v>2013</v>
       </c>
       <c r="C227" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D227" t="s">
         <v>151</v>
@@ -12513,7 +12513,7 @@
         <v>2016</v>
       </c>
       <c r="C228" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D228" t="s">
         <v>151</v>
@@ -12533,13 +12533,13 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B229">
         <v>1981</v>
       </c>
       <c r="C229" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D229" t="s">
         <v>125</v>
@@ -12551,7 +12551,7 @@
         <v>14755</v>
       </c>
       <c r="G229" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I229" t="s">
         <v>194</v>
@@ -12559,13 +12559,13 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B230">
         <v>1985</v>
       </c>
       <c r="C230" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D230" t="s">
         <v>86</v>
@@ -12577,7 +12577,7 @@
         <v>7563</v>
       </c>
       <c r="G230" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I230" t="s">
         <v>194</v>
@@ -12585,16 +12585,16 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B231">
         <v>1989</v>
       </c>
       <c r="C231" t="s">
+        <v>236</v>
+      </c>
+      <c r="D231" t="s">
         <v>239</v>
-      </c>
-      <c r="D231" t="s">
-        <v>242</v>
       </c>
       <c r="E231" s="79" t="s">
         <v>70</v>
@@ -12603,7 +12603,7 @@
         <v>14450</v>
       </c>
       <c r="G231" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I231" t="s">
         <v>194</v>
@@ -12611,16 +12611,16 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B232">
         <v>1995</v>
       </c>
       <c r="C232" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D232" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E232" s="79" t="s">
         <v>70</v>
@@ -12629,7 +12629,7 @@
         <v>6819</v>
       </c>
       <c r="G232" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I232" t="s">
         <v>194</v>
@@ -12637,16 +12637,16 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B233">
         <v>2001</v>
       </c>
       <c r="C233" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D233" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E233" s="79" t="s">
         <v>70</v>
@@ -12655,7 +12655,7 @@
         <v>6786</v>
       </c>
       <c r="G233" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I233" t="s">
         <v>194</v>
@@ -12663,16 +12663,16 @@
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B234">
         <v>2003</v>
       </c>
       <c r="C234" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D234" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E234" s="79" t="s">
         <v>70</v>
@@ -12681,7 +12681,7 @@
         <v>10210</v>
       </c>
       <c r="G234" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I234" t="s">
         <v>194</v>
@@ -12689,16 +12689,16 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B235">
         <v>2004</v>
       </c>
       <c r="C235" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D235" t="s">
-        <v>243</v>
+        <v>331</v>
       </c>
       <c r="E235" s="79" t="s">
         <v>70</v>
@@ -12707,7 +12707,7 @@
         <v>11361</v>
       </c>
       <c r="G235" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I235" t="s">
         <v>194</v>
@@ -12715,16 +12715,16 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B236">
         <v>2008</v>
       </c>
       <c r="C236" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D236" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E236" s="79" t="s">
         <v>70</v>
@@ -12733,7 +12733,7 @@
         <v>9345</v>
       </c>
       <c r="G236" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I236" t="s">
         <v>194</v>
@@ -12741,16 +12741,16 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B237">
         <v>2010</v>
       </c>
       <c r="C237" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D237" t="s">
-        <v>243</v>
+        <v>331</v>
       </c>
       <c r="E237" s="79" t="s">
         <v>70</v>
@@ -12759,7 +12759,7 @@
         <v>18071</v>
       </c>
       <c r="G237" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I237" t="s">
         <v>194</v>
@@ -12767,16 +12767,16 @@
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B238">
         <v>2014</v>
       </c>
       <c r="C238" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D238" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E238" s="79" t="s">
         <v>70</v>
@@ -12785,7 +12785,7 @@
         <v>14162</v>
       </c>
       <c r="G238" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I238" t="s">
         <v>194</v>
@@ -12799,7 +12799,7 @@
         <v>1994</v>
       </c>
       <c r="C239" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D239" t="s">
         <v>154</v>
@@ -12825,7 +12825,7 @@
         <v>1997</v>
       </c>
       <c r="C240" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D240" t="s">
         <v>154</v>
@@ -12851,10 +12851,10 @@
         <v>1998</v>
       </c>
       <c r="C241" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D241" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E241" s="79" t="s">
         <v>70</v>
@@ -12877,10 +12877,10 @@
         <v>2000</v>
       </c>
       <c r="C242" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D242" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E242" s="79" t="s">
         <v>70</v>
@@ -12903,10 +12903,10 @@
         <v>2004</v>
       </c>
       <c r="C243" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D243" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E243" s="79" t="s">
         <v>70</v>
@@ -12929,10 +12929,10 @@
         <v>2007</v>
       </c>
       <c r="C244" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D244" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E244" s="79" t="s">
         <v>70</v>
@@ -12955,10 +12955,10 @@
         <v>2010</v>
       </c>
       <c r="C245" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D245" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E245" s="79" t="s">
         <v>70</v>
@@ -12981,10 +12981,10 @@
         <v>2013</v>
       </c>
       <c r="C246" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D246" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E246" s="79" t="s">
         <v>70</v>
@@ -13001,16 +13001,16 @@
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B247">
         <v>1997</v>
       </c>
       <c r="C247" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D247" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E247" s="79" t="s">
         <v>70</v>
@@ -13019,7 +13019,7 @@
         <v>5230</v>
       </c>
       <c r="G247" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I247" t="s">
         <v>194</v>
@@ -13027,16 +13027,16 @@
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B248">
         <v>2001</v>
       </c>
       <c r="C248" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D248" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E248" s="79" t="s">
         <v>70</v>
@@ -13045,7 +13045,7 @@
         <v>5787</v>
       </c>
       <c r="G248" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I248" t="s">
         <v>194</v>
@@ -13053,16 +13053,16 @@
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B249">
         <v>2005</v>
       </c>
       <c r="C249" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D249" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E249" s="79" t="s">
         <v>70</v>
@@ -13071,7 +13071,7 @@
         <v>6272</v>
       </c>
       <c r="G249" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I249" t="s">
         <v>194</v>
@@ -13079,16 +13079,16 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B250">
         <v>2007</v>
       </c>
       <c r="C250" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D250" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E250" s="79" t="s">
         <v>70</v>
@@ -13097,7 +13097,7 @@
         <v>6173</v>
       </c>
       <c r="G250" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I250" t="s">
         <v>194</v>
@@ -13105,16 +13105,16 @@
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B251">
         <v>2010</v>
       </c>
       <c r="C251" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D251" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E251" s="79" t="s">
         <v>70</v>
@@ -13123,7 +13123,7 @@
         <v>6168</v>
       </c>
       <c r="G251" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I251" t="s">
         <v>194</v>
@@ -13131,16 +13131,16 @@
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B252">
         <v>2012</v>
       </c>
       <c r="C252" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D252" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E252" s="79" t="s">
         <v>70</v>
@@ -13149,7 +13149,7 @@
         <v>8742</v>
       </c>
       <c r="G252" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I252" t="s">
         <v>194</v>
@@ -13157,16 +13157,16 @@
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B253">
         <v>2014</v>
       </c>
       <c r="C253" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D253" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E253" s="79" t="s">
         <v>70</v>
@@ -13175,7 +13175,7 @@
         <v>8465</v>
       </c>
       <c r="G253" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I253" t="s">
         <v>194</v>
@@ -13183,16 +13183,16 @@
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B254">
         <v>2016</v>
       </c>
       <c r="C254" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D254" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E254" s="79" t="s">
         <v>70</v>
@@ -13201,7 +13201,7 @@
         <v>8903</v>
       </c>
       <c r="G254" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I254" t="s">
         <v>194</v>
@@ -13215,7 +13215,7 @@
         <v>2008</v>
       </c>
       <c r="C255" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D255" t="s">
         <v>157</v>
@@ -13235,16 +13235,16 @@
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B256">
         <v>2006</v>
       </c>
       <c r="C256" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D256" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="E256" s="79" t="s">
         <v>70</v>
@@ -13253,7 +13253,7 @@
         <v>15532</v>
       </c>
       <c r="G256" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="I256" t="s">
         <v>194</v>
@@ -13261,16 +13261,16 @@
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B257">
         <v>2008</v>
       </c>
       <c r="C257" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D257" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="E257" s="79" t="s">
         <v>70</v>
@@ -13279,7 +13279,7 @@
         <v>13655</v>
       </c>
       <c r="G257" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="I257" t="s">
         <v>194</v>
@@ -13287,16 +13287,16 @@
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B258">
         <v>2010</v>
       </c>
       <c r="C258" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D258" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="E258" s="79" t="s">
         <v>70</v>
@@ -13305,7 +13305,7 @@
         <v>13317</v>
       </c>
       <c r="G258" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="I258" t="s">
         <v>194</v>
@@ -13313,16 +13313,16 @@
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B259">
         <v>2012</v>
       </c>
       <c r="C259" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D259" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="E259" s="79" t="s">
         <v>70</v>
@@ -13331,7 +13331,7 @@
         <v>13075</v>
       </c>
       <c r="G259" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="I259" t="s">
         <v>194</v>
@@ -13345,7 +13345,7 @@
         <v>1986</v>
       </c>
       <c r="C260" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D260" t="s">
         <v>160</v>
@@ -13371,7 +13371,7 @@
         <v>1991</v>
       </c>
       <c r="C261" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D261" t="s">
         <v>160</v>
@@ -13397,7 +13397,7 @@
         <v>1994</v>
       </c>
       <c r="C262" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D262" t="s">
         <v>160</v>
@@ -13423,7 +13423,7 @@
         <v>1997</v>
       </c>
       <c r="C263" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D263" t="s">
         <v>160</v>
@@ -13449,7 +13449,7 @@
         <v>2000</v>
       </c>
       <c r="C264" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D264" t="s">
         <v>160</v>
@@ -13475,7 +13475,7 @@
         <v>2004</v>
       </c>
       <c r="C265" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D265" t="s">
         <v>160</v>
@@ -13501,7 +13501,7 @@
         <v>2007</v>
       </c>
       <c r="C266" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D266" t="s">
         <v>160</v>
@@ -13527,7 +13527,7 @@
         <v>2010</v>
       </c>
       <c r="C267" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D267" t="s">
         <v>160</v>
@@ -13553,7 +13553,7 @@
         <v>2013</v>
       </c>
       <c r="C268" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D268" t="s">
         <v>160</v>
@@ -13579,7 +13579,7 @@
         <v>2016</v>
       </c>
       <c r="C269" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D269" t="s">
         <v>160</v>
@@ -13599,16 +13599,16 @@
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B270">
         <v>2006</v>
       </c>
       <c r="C270" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D270" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E270" s="79" t="s">
         <v>70</v>
@@ -13617,7 +13617,7 @@
         <v>118590</v>
       </c>
       <c r="G270" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I270" t="s">
         <v>194</v>
@@ -13625,16 +13625,16 @@
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B271">
         <v>2009</v>
       </c>
       <c r="C271" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D271" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E271" s="79" t="s">
         <v>70</v>
@@ -13643,7 +13643,7 @@
         <v>121163</v>
       </c>
       <c r="G271" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I271" t="s">
         <v>194</v>
@@ -13651,16 +13651,16 @@
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B272">
         <v>2011</v>
       </c>
       <c r="C272" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D272" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E272" s="79" t="s">
         <v>70</v>
@@ -13669,7 +13669,7 @@
         <v>111986</v>
       </c>
       <c r="G272" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I272" t="s">
         <v>194</v>
@@ -13677,16 +13677,16 @@
     </row>
     <row r="273" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B273">
         <v>2013</v>
       </c>
       <c r="C273" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D273" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E273" s="79" t="s">
         <v>70</v>
@@ -13695,7 +13695,7 @@
         <v>116543</v>
       </c>
       <c r="G273" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I273" t="s">
         <v>194</v>
@@ -13703,16 +13703,16 @@
     </row>
     <row r="274" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B274">
         <v>2016</v>
       </c>
       <c r="C274" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D274" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E274" s="79" t="s">
         <v>70</v>
@@ -13721,7 +13721,7 @@
         <v>148199</v>
       </c>
       <c r="G274" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I274" t="s">
         <v>194</v>
@@ -13729,16 +13729,16 @@
     </row>
     <row r="275" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B275">
         <v>1990</v>
       </c>
       <c r="C275" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D275" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E275" s="79" t="s">
         <v>70</v>
@@ -13747,7 +13747,7 @@
         <v>25793</v>
       </c>
       <c r="G275" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I275" t="s">
         <v>194</v>
@@ -13755,16 +13755,16 @@
     </row>
     <row r="276" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B276">
         <v>1992</v>
       </c>
       <c r="C276" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D276" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E276" s="79" t="s">
         <v>70</v>
@@ -13773,7 +13773,7 @@
         <v>35948</v>
       </c>
       <c r="G276" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I276" t="s">
         <v>194</v>
@@ -13781,16 +13781,16 @@
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B277">
         <v>1994</v>
       </c>
       <c r="C277" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D277" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E277" s="79" t="s">
         <v>70</v>
@@ -13799,7 +13799,7 @@
         <v>45379</v>
       </c>
       <c r="G277" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I277" t="s">
         <v>194</v>
@@ -13807,16 +13807,16 @@
     </row>
     <row r="278" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B278">
         <v>1996</v>
       </c>
       <c r="C278" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D278" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E278" s="79" t="s">
         <v>70</v>
@@ -13825,7 +13825,7 @@
         <v>33636</v>
       </c>
       <c r="G278" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I278" t="s">
         <v>194</v>
@@ -13833,16 +13833,16 @@
     </row>
     <row r="279" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B279">
         <v>1998</v>
       </c>
       <c r="C279" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D279" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E279" s="79" t="s">
         <v>70</v>
@@ -13851,7 +13851,7 @@
         <v>48107</v>
       </c>
       <c r="G279" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I279" t="s">
         <v>194</v>
@@ -13859,16 +13859,16 @@
     </row>
     <row r="280" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B280">
         <v>2000</v>
       </c>
       <c r="C280" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D280" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E280" s="79" t="s">
         <v>70</v>
@@ -13877,7 +13877,7 @@
         <v>65036</v>
       </c>
       <c r="G280" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I280" t="s">
         <v>194</v>
@@ -13885,16 +13885,16 @@
     </row>
     <row r="281" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B281" s="80">
         <v>2003</v>
       </c>
       <c r="C281" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D281" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E281" s="79" t="s">
         <v>70</v>
@@ -13903,7 +13903,7 @@
         <v>68153</v>
       </c>
       <c r="G281" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="H281" s="78"/>
       <c r="I281" t="s">
@@ -13916,16 +13916,16 @@
     </row>
     <row r="282" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B282" s="80">
         <v>2006</v>
       </c>
       <c r="C282" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D282" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E282" s="79" t="s">
         <v>70</v>
@@ -13934,7 +13934,7 @@
         <v>73720</v>
       </c>
       <c r="G282" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I282" t="s">
         <v>194</v>
@@ -13942,16 +13942,16 @@
     </row>
     <row r="283" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B283">
         <v>2009</v>
       </c>
       <c r="C283" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D283" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E283" s="79" t="s">
         <v>70</v>
@@ -13960,7 +13960,7 @@
         <v>71460</v>
       </c>
       <c r="G283" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I283" t="s">
         <v>194</v>
@@ -13968,16 +13968,16 @@
     </row>
     <row r="284" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B284">
         <v>2011</v>
       </c>
       <c r="C284" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D284" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E284" s="79" t="s">
         <v>70</v>
@@ -13986,7 +13986,7 @@
         <v>59084</v>
       </c>
       <c r="G284" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="H284" s="78"/>
       <c r="I284" t="s">
@@ -13997,16 +13997,16 @@
     </row>
     <row r="285" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B285" s="80">
         <v>2013</v>
       </c>
       <c r="C285" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D285" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E285" s="79" t="s">
         <v>70</v>
@@ -14015,7 +14015,7 @@
         <v>66725</v>
       </c>
       <c r="G285" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I285" t="s">
         <v>194</v>
@@ -14023,16 +14023,16 @@
     </row>
     <row r="286" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B286">
         <v>2015</v>
       </c>
       <c r="C286" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D286" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E286" s="79" t="s">
         <v>70</v>
@@ -14041,7 +14041,7 @@
         <v>83887</v>
       </c>
       <c r="G286" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I286" t="s">
         <v>194</v>
@@ -14049,16 +14049,16 @@
     </row>
     <row r="287" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B287">
         <v>2017</v>
       </c>
       <c r="C287" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D287" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E287" s="79" t="s">
         <v>70</v>
@@ -14067,7 +14067,7 @@
         <v>70948</v>
       </c>
       <c r="G287" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I287" t="s">
         <v>194</v>
@@ -14075,16 +14075,16 @@
     </row>
     <row r="288" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B288">
         <v>2002</v>
       </c>
       <c r="C288" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D288" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E288" s="79" t="s">
         <v>70</v>
@@ -14093,7 +14093,7 @@
         <v>17124</v>
       </c>
       <c r="G288" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="I288" t="s">
         <v>194</v>
@@ -14101,16 +14101,16 @@
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B289">
         <v>2013</v>
       </c>
       <c r="C289" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D289" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E289" s="79" t="s">
         <v>70</v>
@@ -14119,7 +14119,7 @@
         <v>17890</v>
       </c>
       <c r="G289" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="I289" t="s">
         <v>194</v>
@@ -14127,16 +14127,16 @@
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B290" s="80">
         <v>2004</v>
       </c>
       <c r="C290" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D290" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E290" s="79" t="s">
         <v>70</v>
@@ -14145,7 +14145,7 @@
         <v>12510</v>
       </c>
       <c r="G290" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="I290" t="s">
         <v>194</v>
@@ -14153,16 +14153,16 @@
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B291" s="80">
         <v>2007</v>
       </c>
       <c r="C291" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D291" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E291" s="79" t="s">
         <v>70</v>
@@ -14171,7 +14171,7 @@
         <v>219978</v>
       </c>
       <c r="G291" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="I291" t="s">
         <v>194</v>
@@ -14179,16 +14179,16 @@
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B292" s="80">
         <v>2010</v>
       </c>
       <c r="C292" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D292" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E292" s="79" t="s">
         <v>70</v>
@@ -14197,7 +14197,7 @@
         <v>226261</v>
       </c>
       <c r="G292" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="I292" t="s">
         <v>194</v>
@@ -14205,16 +14205,16 @@
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B293" s="80">
         <v>2013</v>
       </c>
       <c r="C293" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D293" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E293" s="79" t="s">
         <v>70</v>
@@ -14223,7 +14223,7 @@
         <v>228944</v>
       </c>
       <c r="G293" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="I293" t="s">
         <v>194</v>
@@ -14231,16 +14231,16 @@
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B294" s="80">
         <v>2016</v>
       </c>
       <c r="C294" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D294" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E294" s="79" t="s">
         <v>70</v>
@@ -14249,7 +14249,7 @@
         <v>231178</v>
       </c>
       <c r="G294" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="I294" t="s">
         <v>194</v>
@@ -14257,16 +14257,16 @@
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B295">
         <v>2007</v>
       </c>
       <c r="C295" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D295" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E295" s="79" t="s">
         <v>70</v>
@@ -14275,7 +14275,7 @@
         <v>8363</v>
       </c>
       <c r="G295" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="I295" t="s">
         <v>194</v>
@@ -14283,16 +14283,16 @@
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B296">
         <v>2012</v>
       </c>
       <c r="C296" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D296" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E296" s="79" t="s">
         <v>70</v>
@@ -14301,7 +14301,7 @@
         <v>12060</v>
       </c>
       <c r="G296" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I296" t="s">
         <v>194</v>
@@ -14309,13 +14309,13 @@
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B297" s="80">
         <v>2010</v>
       </c>
       <c r="C297" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D297" t="s">
         <v>125</v>
@@ -14327,7 +14327,7 @@
         <v>5669</v>
       </c>
       <c r="G297" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="I297" t="s">
         <v>194</v>
@@ -14335,13 +14335,13 @@
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B298" s="80">
         <v>2013</v>
       </c>
       <c r="C298" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D298" t="s">
         <v>125</v>
@@ -14353,7 +14353,7 @@
         <v>2827</v>
       </c>
       <c r="G298" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="I298" t="s">
         <v>194</v>
@@ -14361,13 +14361,13 @@
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B299" s="80">
         <v>2016</v>
       </c>
       <c r="C299" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D299" t="s">
         <v>125</v>
@@ -14379,7 +14379,7 @@
         <v>2768</v>
       </c>
       <c r="G299" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="I299" t="s">
         <v>194</v>
@@ -14387,16 +14387,16 @@
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B300" s="80">
         <v>2006</v>
       </c>
       <c r="C300" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D300" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E300" s="79" t="s">
         <v>70</v>
@@ -14405,7 +14405,7 @@
         <v>13686</v>
       </c>
       <c r="G300" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="I300" t="s">
         <v>194</v>
@@ -14413,16 +14413,16 @@
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B301" s="80">
         <v>2011</v>
       </c>
       <c r="C301" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D301" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E301" s="79" t="s">
         <v>70</v>
@@ -14431,7 +14431,7 @@
         <v>13482</v>
       </c>
       <c r="G301" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="I301" t="s">
         <v>194</v>
@@ -14439,16 +14439,16 @@
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B302" s="80">
         <v>2014</v>
       </c>
       <c r="C302" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D302" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E302" s="79" t="s">
         <v>70</v>
@@ -14457,7 +14457,7 @@
         <v>11536</v>
       </c>
       <c r="G302" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="I302" t="s">
         <v>194</v>
@@ -14465,16 +14465,16 @@
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B303">
         <v>2004</v>
       </c>
       <c r="C303" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D303" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E303" s="79" t="s">
         <v>70</v>
@@ -14483,7 +14483,7 @@
         <v>41554</v>
       </c>
       <c r="G303" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I303" t="s">
         <v>194</v>
@@ -14491,16 +14491,16 @@
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B304">
         <v>2011</v>
       </c>
       <c r="C304" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D304" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E304" s="79" t="s">
         <v>70</v>
@@ -14509,7 +14509,7 @@
         <v>42152</v>
       </c>
       <c r="G304" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I304" t="s">
         <v>194</v>
@@ -14517,16 +14517,16 @@
     </row>
     <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B305" s="80">
         <v>2002</v>
       </c>
       <c r="C305" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D305" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E305" s="79" t="s">
         <v>70</v>
@@ -14535,7 +14535,7 @@
         <v>10800</v>
       </c>
       <c r="G305" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I305" t="s">
         <v>194</v>
@@ -14543,16 +14543,16 @@
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B306" s="80">
         <v>2008</v>
       </c>
       <c r="C306" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D306" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E306" s="79" t="s">
         <v>70</v>
@@ -14561,7 +14561,7 @@
         <v>12600</v>
       </c>
       <c r="G306" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I306" t="s">
         <v>194</v>
@@ -14569,16 +14569,16 @@
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B307" s="80">
         <v>2015</v>
       </c>
       <c r="C307" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D307" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E307" s="79" t="s">
         <v>70</v>
@@ -14587,7 +14587,7 @@
         <v>12899</v>
       </c>
       <c r="G307" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I307" t="s">
         <v>194</v>
@@ -14595,16 +14595,16 @@
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B308">
         <v>1984</v>
       </c>
       <c r="C308" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D308" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E308" s="79" t="s">
         <v>70</v>
@@ -14613,7 +14613,7 @@
         <v>4735</v>
       </c>
       <c r="G308" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="I308" t="s">
         <v>194</v>
@@ -14621,16 +14621,16 @@
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B309">
         <v>1989</v>
       </c>
       <c r="C309" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D309" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E309" s="79" t="s">
         <v>70</v>
@@ -14639,7 +14639,7 @@
         <v>11531</v>
       </c>
       <c r="G309" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="I309" t="s">
         <v>194</v>
@@ -14647,16 +14647,16 @@
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B310">
         <v>1992</v>
       </c>
       <c r="C310" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D310" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E310" s="79" t="s">
         <v>70</v>
@@ -14665,7 +14665,7 @@
         <v>10530</v>
       </c>
       <c r="G310" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="I310" t="s">
         <v>194</v>
@@ -14673,16 +14673,16 @@
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B311">
         <v>1994</v>
       </c>
       <c r="C311" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D311" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E311" s="79" t="s">
         <v>70</v>
@@ -14691,7 +14691,7 @@
         <v>12815</v>
       </c>
       <c r="G311" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I311" t="s">
         <v>194</v>
@@ -14699,16 +14699,16 @@
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B312">
         <v>1996</v>
       </c>
       <c r="C312" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D312" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E312" s="79" t="s">
         <v>70</v>
@@ -14717,7 +14717,7 @@
         <v>14042</v>
       </c>
       <c r="G312" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I312" t="s">
         <v>194</v>
@@ -14725,16 +14725,16 @@
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B313">
         <v>1998</v>
       </c>
       <c r="C313" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D313" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E313" s="79" t="s">
         <v>70</v>
@@ -14743,7 +14743,7 @@
         <v>10952</v>
       </c>
       <c r="G313" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I313" t="s">
         <v>194</v>
@@ -14751,16 +14751,16 @@
     </row>
     <row r="314" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B314">
         <v>2000</v>
       </c>
       <c r="C314" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D314" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E314" s="79" t="s">
         <v>70</v>
@@ -14769,7 +14769,7 @@
         <v>10108</v>
       </c>
       <c r="G314" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I314" t="s">
         <v>194</v>
@@ -14777,16 +14777,16 @@
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B315">
         <v>2002</v>
       </c>
       <c r="C315" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D315" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E315" s="79" t="s">
         <v>70</v>
@@ -14795,7 +14795,7 @@
         <v>17167</v>
       </c>
       <c r="G315" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I315" t="s">
         <v>194</v>
@@ -14803,16 +14803,16 @@
     </row>
     <row r="316" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B316" s="80">
         <v>2004</v>
       </c>
       <c r="C316" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D316" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E316" s="79" t="s">
         <v>70</v>
@@ -14821,7 +14821,7 @@
         <v>9356</v>
       </c>
       <c r="G316" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I316" t="s">
         <v>194</v>
@@ -14829,16 +14829,16 @@
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B317" s="80">
         <v>2008</v>
       </c>
       <c r="C317" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D317" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E317" s="79" t="s">
         <v>70</v>
@@ -14847,7 +14847,7 @@
         <v>10337</v>
       </c>
       <c r="G317" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I317" t="s">
         <v>194</v>
@@ -14855,16 +14855,16 @@
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B318" s="80">
         <v>2010</v>
       </c>
       <c r="C318" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D318" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E318" s="79" t="s">
         <v>70</v>
@@ -14873,7 +14873,7 @@
         <v>27655</v>
       </c>
       <c r="G318" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I318" t="s">
         <v>194</v>
@@ -14881,16 +14881,16 @@
     </row>
     <row r="319" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B319">
         <v>2012</v>
       </c>
       <c r="C319" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D319" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E319" s="79" t="s">
         <v>70</v>
@@ -14899,7 +14899,7 @@
         <v>9002</v>
       </c>
       <c r="G319" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I319" t="s">
         <v>194</v>
@@ -14907,16 +14907,16 @@
     </row>
     <row r="320" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B320">
         <v>2014</v>
       </c>
       <c r="C320" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D320" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E320" s="79" t="s">
         <v>70</v>
@@ -14925,7 +14925,7 @@
         <v>19479</v>
       </c>
       <c r="G320" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I320" t="s">
         <v>194</v>
@@ -14933,16 +14933,16 @@
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B321" s="80">
         <v>2016</v>
       </c>
       <c r="C321" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D321" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E321" s="79" t="s">
         <v>70</v>
@@ -14951,7 +14951,7 @@
         <v>70311</v>
       </c>
       <c r="G321" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I321" t="s">
         <v>194</v>
@@ -14959,16 +14959,16 @@
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B322" s="80">
         <v>2018</v>
       </c>
       <c r="C322" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D322" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E322" s="79" t="s">
         <v>70</v>
@@ -14977,7 +14977,7 @@
         <v>74647</v>
       </c>
       <c r="G322" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I322" t="s">
         <v>194</v>
@@ -14985,16 +14985,16 @@
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B323" s="80">
         <v>2007</v>
       </c>
       <c r="C323" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D323" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E323" s="79" t="s">
         <v>70</v>
@@ -15003,7 +15003,7 @@
         <v>13091</v>
       </c>
       <c r="G323" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="I323" t="s">
         <v>194</v>
@@ -15011,16 +15011,16 @@
     </row>
     <row r="324" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B324" s="80">
         <v>2010</v>
       </c>
       <c r="C324" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D324" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E324" s="79" t="s">
         <v>70</v>
@@ -15029,7 +15029,7 @@
         <v>13391</v>
       </c>
       <c r="G324" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="I324" t="s">
         <v>194</v>
@@ -15037,16 +15037,16 @@
     </row>
     <row r="325" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B325" s="80">
         <v>2013</v>
       </c>
       <c r="C325" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D325" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E325" s="79" t="s">
         <v>70</v>
@@ -15055,7 +15055,7 @@
         <v>11905</v>
       </c>
       <c r="G325" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="I325" t="s">
         <v>194</v>
@@ -15063,16 +15063,16 @@
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B326">
         <v>2000</v>
       </c>
       <c r="C326" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D326" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E326" s="79" t="s">
         <v>70</v>
@@ -15081,7 +15081,7 @@
         <v>8131</v>
       </c>
       <c r="G326" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I326" t="s">
         <v>194</v>
@@ -15089,16 +15089,16 @@
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B327">
         <v>2004</v>
       </c>
       <c r="C327" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D327" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E327" s="79" t="s">
         <v>70</v>
@@ -15107,7 +15107,7 @@
         <v>7823</v>
       </c>
       <c r="G327" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I327" t="s">
         <v>194</v>
@@ -15115,16 +15115,16 @@
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B328">
         <v>2007</v>
       </c>
       <c r="C328" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D328" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E328" s="79" t="s">
         <v>70</v>
@@ -15133,7 +15133,7 @@
         <v>4812</v>
       </c>
       <c r="G328" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I328" t="s">
         <v>194</v>
@@ -15141,16 +15141,16 @@
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B329">
         <v>2010</v>
       </c>
       <c r="C329" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D329" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E329" s="79" t="s">
         <v>70</v>
@@ -15159,7 +15159,7 @@
         <v>5003</v>
       </c>
       <c r="G329" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I329" t="s">
         <v>194</v>
@@ -15167,16 +15167,16 @@
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B330">
         <v>2013</v>
       </c>
       <c r="C330" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D330" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E330" s="79" t="s">
         <v>70</v>
@@ -15185,7 +15185,7 @@
         <v>5424</v>
       </c>
       <c r="G330" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I330" t="s">
         <v>194</v>
@@ -15193,16 +15193,16 @@
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B331">
         <v>2016</v>
       </c>
       <c r="C331" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D331" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E331" s="79" t="s">
         <v>70</v>
@@ -15211,7 +15211,7 @@
         <v>10219</v>
       </c>
       <c r="G331" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I331" t="s">
         <v>194</v>
@@ -15219,16 +15219,16 @@
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B332" s="80">
         <v>2004</v>
       </c>
       <c r="C332" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D332" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E332" s="79" t="s">
         <v>70</v>
@@ -15237,7 +15237,7 @@
         <v>19502</v>
       </c>
       <c r="G332" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="I332" t="s">
         <v>194</v>
@@ -15245,16 +15245,16 @@
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B333" s="80">
         <v>2007</v>
       </c>
       <c r="C333" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D333" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E333" s="79" t="s">
         <v>70</v>
@@ -15263,7 +15263,7 @@
         <v>22204</v>
       </c>
       <c r="G333" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="I333" t="s">
         <v>194</v>
@@ -15271,16 +15271,16 @@
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B334" s="80">
         <v>2010</v>
       </c>
       <c r="C334" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D334" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E334" s="79" t="s">
         <v>70</v>
@@ -15289,7 +15289,7 @@
         <v>21496</v>
       </c>
       <c r="G334" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="I334" t="s">
         <v>194</v>
@@ -15297,16 +15297,16 @@
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B335" s="80">
         <v>2013</v>
       </c>
       <c r="C335" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D335" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E335" s="79" t="s">
         <v>70</v>
@@ -15315,7 +15315,7 @@
         <v>30453</v>
       </c>
       <c r="G335" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="I335" t="s">
         <v>194</v>
@@ -15323,16 +15323,16 @@
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B336" s="80">
         <v>2016</v>
       </c>
       <c r="C336" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D336" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E336" s="79" t="s">
         <v>70</v>
@@ -15341,7 +15341,7 @@
         <v>35785</v>
       </c>
       <c r="G336" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="I336" t="s">
         <v>194</v>
@@ -15349,16 +15349,16 @@
     </row>
     <row r="337" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B337" s="80">
         <v>2000</v>
       </c>
       <c r="C337" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D337" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E337" s="79" t="s">
         <v>70</v>
@@ -15367,7 +15367,7 @@
         <v>3319</v>
       </c>
       <c r="G337" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I337" t="s">
         <v>194</v>
@@ -15375,16 +15375,16 @@
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B338" s="80">
         <v>2004</v>
       </c>
       <c r="C338" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D338" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E338" s="79" t="s">
         <v>70</v>
@@ -15393,7 +15393,7 @@
         <v>3394</v>
       </c>
       <c r="G338" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I338" t="s">
         <v>194</v>
@@ -15401,16 +15401,16 @@
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B339" s="80">
         <v>2007</v>
       </c>
       <c r="C339" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D339" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E339" s="79" t="s">
         <v>70</v>
@@ -15419,7 +15419,7 @@
         <v>3933</v>
       </c>
       <c r="G339" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I339" t="s">
         <v>194</v>
@@ -15427,16 +15427,16 @@
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B340">
         <v>2010</v>
       </c>
       <c r="C340" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D340" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E340" s="79" t="s">
         <v>70</v>
@@ -15445,7 +15445,7 @@
         <v>6323</v>
       </c>
       <c r="G340" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I340" t="s">
         <v>194</v>
@@ -15453,16 +15453,16 @@
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B341">
         <v>2011</v>
       </c>
       <c r="C341" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D341" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E341" s="79" t="s">
         <v>70</v>
@@ -15471,7 +15471,7 @@
         <v>9990</v>
       </c>
       <c r="G341" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I341" t="s">
         <v>194</v>
@@ -15479,16 +15479,16 @@
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B342">
         <v>2013</v>
       </c>
       <c r="C342" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D342" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E342" s="79" t="s">
         <v>70</v>
@@ -15497,7 +15497,7 @@
         <v>45000</v>
       </c>
       <c r="G342" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I342" t="s">
         <v>194</v>
@@ -15505,16 +15505,16 @@
     </row>
     <row r="343" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B343">
         <v>2014</v>
       </c>
       <c r="C343" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D343" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E343" s="79" t="s">
         <v>70</v>
@@ -15523,7 +15523,7 @@
         <v>45000</v>
       </c>
       <c r="G343" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I343" t="s">
         <v>194</v>
@@ -15531,16 +15531,16 @@
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B344">
         <v>2015</v>
       </c>
       <c r="C344" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D344" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E344" s="79" t="s">
         <v>70</v>
@@ -15549,7 +15549,7 @@
         <v>60000</v>
       </c>
       <c r="G344" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I344" t="s">
         <v>194</v>
@@ -15557,16 +15557,16 @@
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B345">
         <v>2016</v>
       </c>
       <c r="C345" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D345" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E345" s="79" t="s">
         <v>70</v>
@@ -15575,7 +15575,7 @@
         <v>160008</v>
       </c>
       <c r="G345" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I345" t="s">
         <v>194</v>
@@ -15583,16 +15583,16 @@
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B346" s="80">
         <v>2008</v>
       </c>
       <c r="C346" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D346" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E346" s="79" t="s">
         <v>70</v>
@@ -15601,7 +15601,7 @@
         <v>7296</v>
       </c>
       <c r="G346" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I346" t="s">
         <v>194</v>
@@ -15609,16 +15609,16 @@
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B347" s="80">
         <v>2010</v>
       </c>
       <c r="C347" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D347" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E347" s="79" t="s">
         <v>70</v>
@@ -15627,7 +15627,7 @@
         <v>6786</v>
       </c>
       <c r="G347" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I347" t="s">
         <v>194</v>
@@ -15635,16 +15635,16 @@
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B348" s="80">
         <v>2012</v>
       </c>
       <c r="C348" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D348" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E348" s="79" t="s">
         <v>70</v>
@@ -15653,7 +15653,7 @@
         <v>8040</v>
       </c>
       <c r="G348" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I348" t="s">
         <v>194</v>
@@ -15947,16 +15947,16 @@
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B360" s="80">
         <v>2004</v>
       </c>
       <c r="C360" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D360" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E360" s="79" t="s">
         <v>70</v>
@@ -15965,7 +15965,7 @@
         <v>18392</v>
       </c>
       <c r="G360" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="I360" t="s">
         <v>194</v>
@@ -15973,16 +15973,16 @@
     </row>
     <row r="361" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B361" s="80">
         <v>2007</v>
       </c>
       <c r="C361" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D361" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E361" s="79" t="s">
         <v>70</v>
@@ -15991,7 +15991,7 @@
         <v>49136</v>
       </c>
       <c r="G361" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="I361" t="s">
         <v>194</v>
@@ -15999,16 +15999,16 @@
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B362" s="80">
         <v>2010</v>
       </c>
       <c r="C362" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D362" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E362" s="79" t="s">
         <v>70</v>
@@ -16017,7 +16017,7 @@
         <v>46550</v>
       </c>
       <c r="G362" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="I362" t="s">
         <v>194</v>
@@ -16025,16 +16025,16 @@
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B363" s="80">
         <v>2013</v>
       </c>
       <c r="C363" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D363" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E363" s="79" t="s">
         <v>70</v>
@@ -16043,7 +16043,7 @@
         <v>46622</v>
       </c>
       <c r="G363" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="I363" t="s">
         <v>194</v>
@@ -16051,16 +16051,16 @@
     </row>
     <row r="364" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B364" s="80">
         <v>2016</v>
       </c>
       <c r="C364" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D364" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E364" s="79" t="s">
         <v>70</v>
@@ -16069,7 +16069,7 @@
         <v>45158</v>
       </c>
       <c r="G364" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="I364" t="s">
         <v>194</v>
@@ -16077,16 +16077,16 @@
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B365" s="80">
         <v>2011</v>
       </c>
       <c r="C365" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D365" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="E365" s="79" t="s">
         <v>70</v>
@@ -16095,7 +16095,7 @@
         <v>9399</v>
       </c>
       <c r="G365" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="I365" t="s">
         <v>194</v>
@@ -16103,16 +16103,16 @@
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B366" s="80">
         <v>2013</v>
       </c>
       <c r="C366" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D366" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="E366" s="79" t="s">
         <v>70</v>
@@ -16121,14 +16121,13 @@
         <v>9399</v>
       </c>
       <c r="G366" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="I366" t="s">
         <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G119" xr:uid="{02CCEDBC-03D4-44CD-BD29-A9AE77223298}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Updated dofiles & aux Excel file after answers received from LIS
</commit_message>
<xml_diff>
--- a/02.data/_aux/LIS datasets.xlsx
+++ b/02.data/_aux/LIS datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/mviveros_worldbank_org2/Documents/GIT/LIS_data/02.data/_aux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1002" documentId="13_ncr:1_{23E223E5-8195-41FF-8C7D-40BD88F80865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5C6800C-D306-4305-A5D2-758412055C85}"/>
+  <xr:revisionPtr revIDLastSave="1017" documentId="13_ncr:1_{23E223E5-8195-41FF-8C7D-40BD88F80865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF7472D9-1069-4225-B006-E8CCB842AB1C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{DA214762-5DBE-485D-812E-A8355C7FFC9F}"/>
   </bookViews>
@@ -1353,7 +1353,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1387,6 +1387,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1573,7 +1579,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1759,9 +1765,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1769,7 +1782,23 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="68">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -5498,244 +5527,244 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C16:G16 I16:AL16 C2:AL5 C10:AL15 C9:I9 C17:AL21 C22:AD22 AF22:AL22 C23:AL25 C27:AL27 C26:P26 R26:AL26 C7:AL8 C6:AI6 AK6:AL6 K9:U9 W9:Z9">
-    <cfRule type="cellIs" dxfId="65" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="81" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="82" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="84" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ9">
-    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="70" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="71" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="72" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW35">
-    <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="64" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="65" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="66" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ35">
-    <cfRule type="cellIs" dxfId="56" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="61" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="62" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="63" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT35">
-    <cfRule type="cellIs" dxfId="53" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="58" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="59" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="60" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ35">
-    <cfRule type="cellIs" dxfId="50" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="55" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="56" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="57" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO35">
-    <cfRule type="cellIs" dxfId="47" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="52" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="53" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="54" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ35">
-    <cfRule type="cellIs" dxfId="44" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="49" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="50" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="51" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG35">
-    <cfRule type="cellIs" dxfId="41" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="47" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="48" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE35">
-    <cfRule type="cellIs" dxfId="38" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="44" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="45" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA35">
-    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="41" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V35">
-    <cfRule type="cellIs" dxfId="32" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="38" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="39" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q35">
-    <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="35" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB9:AC9">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF9:AG9">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI9">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW33">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT33">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8402,9 +8431,9 @@
   <dimension ref="A1:L660"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C249" sqref="C249"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8463,7 +8492,7 @@
       <c r="E2" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="72">
         <v>14755</v>
       </c>
       <c r="G2" t="s">
@@ -8489,7 +8518,7 @@
       <c r="E3" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="72">
         <v>7563</v>
       </c>
       <c r="G3" t="s">
@@ -8515,7 +8544,7 @@
       <c r="E4" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="72">
         <v>14450</v>
       </c>
       <c r="G4" t="s">
@@ -8541,7 +8570,7 @@
       <c r="E5" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="72">
         <v>6819</v>
       </c>
       <c r="G5" t="s">
@@ -8567,7 +8596,7 @@
       <c r="E6" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="72">
         <v>6786</v>
       </c>
       <c r="G6" t="s">
@@ -8593,7 +8622,7 @@
       <c r="E7" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="72">
         <v>10210</v>
       </c>
       <c r="G7" t="s">
@@ -8619,7 +8648,7 @@
       <c r="E8" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="72">
         <v>11361</v>
       </c>
       <c r="G8" t="s">
@@ -8645,7 +8674,7 @@
       <c r="E9" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="72">
         <v>9345</v>
       </c>
       <c r="G9" t="s">
@@ -8671,7 +8700,7 @@
       <c r="E10" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="72">
         <v>18071</v>
       </c>
       <c r="G10" t="s">
@@ -8697,7 +8726,7 @@
       <c r="E11" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="72">
         <v>14162</v>
       </c>
       <c r="G11" t="s">
@@ -8723,7 +8752,7 @@
       <c r="E12" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="72">
         <v>17768</v>
       </c>
       <c r="G12" t="s">
@@ -8749,7 +8778,7 @@
       <c r="E13" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="72">
         <v>14060</v>
       </c>
       <c r="G13" t="s">
@@ -8763,10 +8792,10 @@
       <c r="A14" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="81">
+      <c r="B14" s="80">
         <v>1987</v>
       </c>
-      <c r="C14" s="80" t="s">
+      <c r="C14" s="79" t="s">
         <v>68</v>
       </c>
       <c r="D14" s="62" t="s">
@@ -10109,7 +10138,7 @@
       <c r="E60" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="72">
         <v>118590</v>
       </c>
       <c r="G60" t="s">
@@ -10135,7 +10164,7 @@
       <c r="E61" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="72">
         <v>121163</v>
       </c>
       <c r="G61" t="s">
@@ -10161,7 +10190,7 @@
       <c r="E62" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="72">
         <v>111986</v>
       </c>
       <c r="G62" t="s">
@@ -10187,7 +10216,7 @@
       <c r="E63" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="72">
         <v>116543</v>
       </c>
       <c r="G63" t="s">
@@ -10213,7 +10242,7 @@
       <c r="E64" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="72">
         <v>148199</v>
       </c>
       <c r="G64" t="s">
@@ -10297,7 +10326,7 @@
       <c r="E67" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="72">
         <v>15136</v>
       </c>
       <c r="G67" t="s">
@@ -10323,7 +10352,7 @@
       <c r="E68" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="72">
         <v>10999</v>
       </c>
       <c r="G68" t="s">
@@ -10349,7 +10378,7 @@
       <c r="E69" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="72">
         <v>20035</v>
       </c>
       <c r="G69" t="s">
@@ -10375,7 +10404,7 @@
       <c r="E70" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="72">
         <v>37475</v>
       </c>
       <c r="G70" t="s">
@@ -10401,7 +10430,7 @@
       <c r="E71" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="72">
         <v>30501</v>
       </c>
       <c r="G71" t="s">
@@ -10427,7 +10456,7 @@
       <c r="E72" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="72">
         <v>30764</v>
       </c>
       <c r="G72" t="s">
@@ -10453,7 +10482,7 @@
       <c r="E73" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="72">
         <v>31218</v>
       </c>
       <c r="G73" t="s">
@@ -10479,7 +10508,7 @@
       <c r="E74" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="72">
         <v>29266</v>
       </c>
       <c r="G74" t="s">
@@ -10505,7 +10534,7 @@
       <c r="E75" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F75">
+      <c r="F75" s="72">
         <v>28970</v>
       </c>
       <c r="G75" t="s">
@@ -10531,7 +10560,7 @@
       <c r="E76" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F76">
+      <c r="F76" s="72">
         <v>29578</v>
       </c>
       <c r="G76" t="s">
@@ -10557,7 +10586,7 @@
       <c r="E77" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F77">
+      <c r="F77" s="72">
         <v>28196</v>
       </c>
       <c r="G77" t="s">
@@ -10583,7 +10612,7 @@
       <c r="E78" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F78">
+      <c r="F78" s="72">
         <v>28589</v>
       </c>
       <c r="G78" t="s">
@@ -10609,7 +10638,7 @@
       <c r="E79" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F79">
+      <c r="F79" s="72">
         <v>27820</v>
       </c>
       <c r="G79" t="s">
@@ -10635,7 +10664,7 @@
       <c r="E80" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F80">
+      <c r="F80" s="72">
         <v>27079</v>
       </c>
       <c r="G80" t="s">
@@ -10661,7 +10690,7 @@
       <c r="E81" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="72">
         <v>27381</v>
       </c>
       <c r="G81" t="s">
@@ -10687,7 +10716,7 @@
       <c r="E82" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="72">
         <v>26745</v>
       </c>
       <c r="G82" t="s">
@@ -10713,7 +10742,7 @@
       <c r="E83" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F83">
+      <c r="F83" s="72">
         <v>25135</v>
       </c>
       <c r="G83" t="s">
@@ -10739,7 +10768,7 @@
       <c r="E84" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="72">
         <v>25690</v>
       </c>
       <c r="G84" t="s">
@@ -10765,7 +10794,7 @@
       <c r="E85" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F85">
+      <c r="F85" s="72">
         <v>25019</v>
       </c>
       <c r="G85" t="s">
@@ -10791,7 +10820,7 @@
       <c r="E86" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="72">
         <v>24231</v>
       </c>
       <c r="G86" t="s">
@@ -10817,7 +10846,7 @@
       <c r="E87" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F87">
+      <c r="F87" s="72">
         <v>24311</v>
       </c>
       <c r="G87" t="s">
@@ -10846,7 +10875,7 @@
       <c r="E88" s="77" t="s">
         <v>331</v>
       </c>
-      <c r="F88">
+      <c r="F88" s="72">
         <v>23014</v>
       </c>
       <c r="G88" t="s">
@@ -10875,7 +10904,7 @@
       <c r="E89" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="72">
         <v>23437</v>
       </c>
       <c r="G89" t="s">
@@ -10904,7 +10933,7 @@
       <c r="E90" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="72">
         <v>25825</v>
       </c>
       <c r="G90" t="s">
@@ -10933,7 +10962,7 @@
       <c r="E91" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F91">
+      <c r="F91" s="72">
         <v>26675</v>
       </c>
       <c r="G91" t="s">
@@ -10962,7 +10991,7 @@
       <c r="E92" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F92">
+      <c r="F92" s="72">
         <v>39769</v>
       </c>
       <c r="G92" t="s">
@@ -10991,7 +11020,7 @@
       <c r="E93" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="72">
         <v>40857</v>
       </c>
       <c r="G93" t="s">
@@ -11136,7 +11165,7 @@
       <c r="E98" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F98">
+      <c r="F98" s="72">
         <v>3270</v>
       </c>
       <c r="G98" t="s">
@@ -11188,7 +11217,7 @@
       <c r="E100" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F100">
+      <c r="F100" s="72">
         <v>6778</v>
       </c>
       <c r="G100" t="s">
@@ -11214,7 +11243,7 @@
       <c r="E101" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F101">
+      <c r="F101" s="72">
         <v>7372</v>
       </c>
       <c r="G101" t="s">
@@ -11240,7 +11269,7 @@
       <c r="E102" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F102">
+      <c r="F102" s="72">
         <v>7513</v>
       </c>
       <c r="G102" t="s">
@@ -11266,7 +11295,7 @@
       <c r="E103" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F103">
+      <c r="F103" s="72">
         <v>7502</v>
       </c>
       <c r="G103" t="s">
@@ -11292,7 +11321,7 @@
       <c r="E104" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F104">
+      <c r="F104" s="72">
         <v>7529</v>
       </c>
       <c r="G104" t="s">
@@ -11318,7 +11347,7 @@
       <c r="E105" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F105">
+      <c r="F105" s="72">
         <v>7341</v>
       </c>
       <c r="G105" t="s">
@@ -11344,7 +11373,7 @@
       <c r="E106" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F106">
+      <c r="F106" s="72">
         <v>6792</v>
       </c>
       <c r="G106" t="s">
@@ -11370,7 +11399,7 @@
       <c r="E107" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F107">
+      <c r="F107" s="72">
         <v>7468</v>
       </c>
       <c r="G107" t="s">
@@ -11396,7 +11425,7 @@
       <c r="E108" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F108">
+      <c r="F108" s="72">
         <v>7762</v>
       </c>
       <c r="G108" t="s">
@@ -11422,7 +11451,7 @@
       <c r="E109" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F109">
+      <c r="F109" s="72">
         <v>8122</v>
       </c>
       <c r="G109" t="s">
@@ -11448,7 +11477,7 @@
       <c r="E110" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F110">
+      <c r="F110" s="72">
         <v>6680</v>
       </c>
       <c r="G110" t="s">
@@ -11474,7 +11503,7 @@
       <c r="E111" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F111">
+      <c r="F111" s="72">
         <v>7341</v>
       </c>
       <c r="G111" t="s">
@@ -11500,7 +11529,7 @@
       <c r="E112" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F112">
+      <c r="F112" s="72">
         <v>25793</v>
       </c>
       <c r="G112" t="s">
@@ -11526,7 +11555,7 @@
       <c r="E113" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F113">
+      <c r="F113" s="72">
         <v>35948</v>
       </c>
       <c r="G113" t="s">
@@ -11552,7 +11581,7 @@
       <c r="E114" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F114">
+      <c r="F114" s="72">
         <v>45379</v>
       </c>
       <c r="G114" t="s">
@@ -11578,7 +11607,7 @@
       <c r="E115" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F115">
+      <c r="F115" s="72">
         <v>33636</v>
       </c>
       <c r="G115" t="s">
@@ -11604,7 +11633,7 @@
       <c r="E116" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F116">
+      <c r="F116" s="72">
         <v>48107</v>
       </c>
       <c r="G116" t="s">
@@ -11630,7 +11659,7 @@
       <c r="E117" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F117">
+      <c r="F117" s="72">
         <v>65036</v>
       </c>
       <c r="G117" t="s">
@@ -11656,7 +11685,7 @@
       <c r="E118" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F118">
+      <c r="F118" s="72">
         <v>68153</v>
       </c>
       <c r="G118" t="s">
@@ -11683,7 +11712,7 @@
       <c r="E119" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F119">
+      <c r="F119" s="72">
         <v>73720</v>
       </c>
       <c r="G119" t="s">
@@ -11709,7 +11738,7 @@
       <c r="E120" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F120">
+      <c r="F120" s="72">
         <v>71460</v>
       </c>
       <c r="G120" t="s">
@@ -11735,7 +11764,7 @@
       <c r="E121" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F121">
+      <c r="F121" s="72">
         <v>59084</v>
       </c>
       <c r="G121" t="s">
@@ -11762,7 +11791,7 @@
       <c r="E122" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F122">
+      <c r="F122" s="72">
         <v>66725</v>
       </c>
       <c r="G122" t="s">
@@ -11788,7 +11817,7 @@
       <c r="E123" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F123">
+      <c r="F123" s="72">
         <v>83887</v>
       </c>
       <c r="G123" t="s">
@@ -11814,7 +11843,7 @@
       <c r="E124" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F124">
+      <c r="F124" s="72">
         <v>70948</v>
       </c>
       <c r="G124" t="s">
@@ -11840,7 +11869,7 @@
       <c r="E125" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F125">
+      <c r="F125" s="72">
         <v>17124</v>
       </c>
       <c r="G125" t="s">
@@ -11866,7 +11895,7 @@
       <c r="E126" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F126">
+      <c r="F126" s="72">
         <v>17890</v>
       </c>
       <c r="G126" t="s">
@@ -11892,7 +11921,7 @@
       <c r="E127" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F127">
+      <c r="F127" s="72">
         <v>20745</v>
       </c>
       <c r="G127" t="s">
@@ -11918,7 +11947,7 @@
       <c r="E128" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F128">
+      <c r="F128" s="72">
         <v>10800</v>
       </c>
       <c r="G128" t="s">
@@ -11944,7 +11973,7 @@
       <c r="E129" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F129">
+      <c r="F129" s="72">
         <v>12600</v>
       </c>
       <c r="G129" t="s">
@@ -11970,7 +11999,7 @@
       <c r="E130" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F130">
+      <c r="F130" s="72">
         <v>12899</v>
       </c>
       <c r="G130" t="s">
@@ -11996,7 +12025,7 @@
       <c r="E131" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F131">
+      <c r="F131" s="72">
         <v>64492</v>
       </c>
       <c r="G131" t="s">
@@ -12022,7 +12051,7 @@
       <c r="E132" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F132">
+      <c r="F132" s="72">
         <v>129164</v>
       </c>
       <c r="G132" t="s">
@@ -12048,7 +12077,7 @@
       <c r="E133" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F133">
+      <c r="F133" s="72">
         <v>132481</v>
       </c>
       <c r="G133" t="s">
@@ -12074,7 +12103,7 @@
       <c r="E134" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F134">
+      <c r="F134" s="72">
         <v>12510</v>
       </c>
       <c r="G134" t="s">
@@ -12100,7 +12129,7 @@
       <c r="E135" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F135">
+      <c r="F135" s="72">
         <v>151402</v>
       </c>
       <c r="G135" t="s">
@@ -12126,7 +12155,7 @@
       <c r="E136" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F136">
+      <c r="F136" s="72">
         <v>77557</v>
       </c>
       <c r="G136" t="s">
@@ -12152,7 +12181,7 @@
       <c r="E137" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F137">
+      <c r="F137" s="72">
         <v>219978</v>
       </c>
       <c r="G137" t="s">
@@ -12178,7 +12207,7 @@
       <c r="E138" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F138">
+      <c r="F138" s="72">
         <v>221988</v>
       </c>
       <c r="G138" t="s">
@@ -12204,7 +12233,7 @@
       <c r="E139" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F139">
+      <c r="F139" s="72">
         <v>221181</v>
       </c>
       <c r="G139" t="s">
@@ -12230,7 +12259,7 @@
       <c r="E140" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F140">
+      <c r="F140" s="72">
         <v>226261</v>
       </c>
       <c r="G140" t="s">
@@ -12256,7 +12285,7 @@
       <c r="E141" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F141">
+      <c r="F141" s="72">
         <v>230269</v>
       </c>
       <c r="G141" t="s">
@@ -12282,7 +12311,7 @@
       <c r="E142" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F142">
+      <c r="F142" s="72">
         <v>228662</v>
       </c>
       <c r="G142" t="s">
@@ -12308,7 +12337,7 @@
       <c r="E143" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F143">
+      <c r="F143" s="72">
         <v>228944</v>
       </c>
       <c r="G143" t="s">
@@ -12334,7 +12363,7 @@
       <c r="E144" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F144">
+      <c r="F144" s="72">
         <v>228932</v>
       </c>
       <c r="G144" t="s">
@@ -12360,7 +12389,7 @@
       <c r="E145" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F145">
+      <c r="F145" s="72">
         <v>232219</v>
       </c>
       <c r="G145" t="s">
@@ -12386,7 +12415,7 @@
       <c r="E146" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F146">
+      <c r="F146" s="72">
         <v>231178</v>
       </c>
       <c r="G146" t="s">
@@ -12412,7 +12441,7 @@
       <c r="E147" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F147">
+      <c r="F147" s="72">
         <v>230909</v>
       </c>
       <c r="G147" t="s">
@@ -12438,7 +12467,7 @@
       <c r="E148" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F148">
+      <c r="F148" s="72">
         <v>231128</v>
       </c>
       <c r="G148" t="s">
@@ -12464,7 +12493,7 @@
       <c r="E149" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F149">
+      <c r="F149" s="72">
         <v>231831</v>
       </c>
       <c r="G149" t="s">
@@ -12490,7 +12519,7 @@
       <c r="E150" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F150">
+      <c r="F150" s="72">
         <v>134399</v>
       </c>
       <c r="G150" t="s">
@@ -12545,7 +12574,7 @@
       <c r="E152" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F152" s="79">
+      <c r="F152" s="72">
         <v>28148</v>
       </c>
       <c r="G152" s="62" t="s">
@@ -12603,7 +12632,7 @@
       <c r="E154" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F154">
+      <c r="F154" s="72">
         <v>4351</v>
       </c>
       <c r="G154" t="s">
@@ -12629,7 +12658,7 @@
       <c r="E155" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F155">
+      <c r="F155" s="72">
         <v>11294</v>
       </c>
       <c r="G155" t="s">
@@ -12655,7 +12684,7 @@
       <c r="E156" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F156">
+      <c r="F156" s="72">
         <v>8866</v>
       </c>
       <c r="G156" t="s">
@@ -12681,7 +12710,7 @@
       <c r="E157" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F157">
+      <c r="F157" s="72">
         <v>8053</v>
       </c>
       <c r="G157" t="s">
@@ -12707,7 +12736,7 @@
       <c r="E158" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F158">
+      <c r="F158" s="72">
         <v>8701</v>
       </c>
       <c r="G158" t="s">
@@ -12776,19 +12805,19 @@
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A161" t="s">
+      <c r="A161" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="82">
         <v>1981</v>
       </c>
-      <c r="C161" s="63" t="s">
+      <c r="C161" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="D161" s="62" t="s">
+      <c r="D161" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="E161" s="59" t="s">
+      <c r="E161" s="84" t="s">
         <v>70</v>
       </c>
       <c r="F161" s="72">
@@ -13139,7 +13168,7 @@
       <c r="E173" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F173">
+      <c r="F173" s="72">
         <v>6768</v>
       </c>
       <c r="G173" t="s">
@@ -13168,7 +13197,7 @@
       <c r="E174" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F174">
+      <c r="F174" s="72">
         <v>6699</v>
       </c>
       <c r="G174" t="s">
@@ -13255,7 +13284,7 @@
       <c r="E177" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F177">
+      <c r="F177" s="72">
         <v>7220</v>
       </c>
       <c r="G177" t="s">
@@ -13284,7 +13313,7 @@
       <c r="E178" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F178">
+      <c r="F178" s="72">
         <v>13082</v>
       </c>
       <c r="G178" t="s">
@@ -13313,7 +13342,7 @@
       <c r="E179" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F179">
+      <c r="F179" s="72">
         <v>11796</v>
       </c>
       <c r="G179" t="s">
@@ -13339,7 +13368,7 @@
       <c r="E180" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F180">
+      <c r="F180" s="72">
         <v>12320</v>
       </c>
       <c r="G180" t="s">
@@ -13365,7 +13394,7 @@
       <c r="E181" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F181">
+      <c r="F181" s="72">
         <v>11909</v>
       </c>
       <c r="G181" t="s">
@@ -13391,7 +13420,7 @@
       <c r="E182" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F182">
+      <c r="F182" s="72">
         <v>11644</v>
       </c>
       <c r="G182" t="s">
@@ -13417,7 +13446,7 @@
       <c r="E183" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F183">
+      <c r="F183" s="72">
         <v>11294</v>
       </c>
       <c r="G183" t="s">
@@ -13443,7 +13472,7 @@
       <c r="E184" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F184">
+      <c r="F184" s="72">
         <v>12361</v>
       </c>
       <c r="G184" t="s">
@@ -13469,7 +13498,7 @@
       <c r="E185" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F185">
+      <c r="F185" s="72">
         <v>11552</v>
       </c>
       <c r="G185" t="s">
@@ -13495,7 +13524,7 @@
       <c r="E186" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F186">
+      <c r="F186" s="72">
         <v>10921</v>
       </c>
       <c r="G186" t="s">
@@ -13521,7 +13550,7 @@
       <c r="E187" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F187">
+      <c r="F187" s="72">
         <v>10270</v>
       </c>
       <c r="G187" t="s">
@@ -13547,7 +13576,7 @@
       <c r="E188" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F188">
+      <c r="F188" s="72">
         <v>13888</v>
       </c>
       <c r="G188" t="s">
@@ -13573,7 +13602,7 @@
       <c r="E189" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F189">
+      <c r="F189" s="72">
         <v>16703</v>
       </c>
       <c r="G189" t="s">
@@ -13599,7 +13628,7 @@
       <c r="E190" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F190">
+      <c r="F190" s="72">
         <v>16397</v>
       </c>
       <c r="G190" t="s">
@@ -13625,7 +13654,7 @@
       <c r="E191" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F191">
+      <c r="F191" s="72">
         <v>17992</v>
       </c>
       <c r="G191" t="s">
@@ -13651,7 +13680,7 @@
       <c r="E192" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F192">
+      <c r="F192" s="72">
         <v>15946</v>
       </c>
       <c r="G192" t="s">
@@ -13677,7 +13706,7 @@
       <c r="E193" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F193">
+      <c r="F193" s="72">
         <v>15908</v>
       </c>
       <c r="G193" t="s">
@@ -13703,7 +13732,7 @@
       <c r="E194" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F194">
+      <c r="F194" s="72">
         <v>14426</v>
       </c>
       <c r="G194" t="s">
@@ -13961,7 +13990,7 @@
       <c r="E203" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F203">
+      <c r="F203" s="72">
         <v>83409</v>
       </c>
       <c r="G203" t="s">
@@ -13987,7 +14016,7 @@
       <c r="E204" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F204">
+      <c r="F204" s="72">
         <v>84669</v>
       </c>
       <c r="G204" t="s">
@@ -14013,7 +14042,7 @@
       <c r="E205" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F205">
+      <c r="F205" s="72">
         <v>85645</v>
       </c>
       <c r="G205" t="s">
@@ -14039,7 +14068,7 @@
       <c r="E206" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F206">
+      <c r="F206" s="72">
         <v>87517</v>
       </c>
       <c r="G206" t="s">
@@ -14065,7 +14094,7 @@
       <c r="E207" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F207">
+      <c r="F207" s="72">
         <v>89245</v>
       </c>
       <c r="G207" t="s">
@@ -14091,7 +14120,7 @@
       <c r="E208" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F208">
+      <c r="F208" s="72">
         <v>8363</v>
       </c>
       <c r="G208" t="s">
@@ -14117,7 +14146,7 @@
       <c r="E209" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F209">
+      <c r="F209" s="72">
         <v>12060</v>
       </c>
       <c r="G209" t="s">
@@ -14288,7 +14317,7 @@
       <c r="E215" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F215">
+      <c r="F215" s="72">
         <v>12996</v>
       </c>
       <c r="G215" t="s">
@@ -14314,7 +14343,7 @@
       <c r="E216" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F216">
+      <c r="F216" s="72">
         <v>13014</v>
       </c>
       <c r="G216" t="s">
@@ -14340,7 +14369,7 @@
       <c r="E217" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F217">
+      <c r="F217" s="72">
         <v>13109</v>
       </c>
       <c r="G217" t="s">
@@ -14366,7 +14395,7 @@
       <c r="E218" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F218">
+      <c r="F218" s="72">
         <v>11965</v>
       </c>
       <c r="G218" t="s">
@@ -14392,7 +14421,7 @@
       <c r="E219" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F219">
+      <c r="F219" s="72">
         <v>13740</v>
       </c>
       <c r="G219" t="s">
@@ -14418,7 +14447,7 @@
       <c r="E220" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F220">
+      <c r="F220" s="72">
         <v>6068</v>
       </c>
       <c r="G220" t="s">
@@ -14444,7 +14473,7 @@
       <c r="E221" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F221">
+      <c r="F221" s="72">
         <v>4169</v>
       </c>
       <c r="G221" t="s">
@@ -14470,7 +14499,7 @@
       <c r="E222" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F222">
+      <c r="F222" s="72">
         <v>4744</v>
       </c>
       <c r="G222" t="s">
@@ -14496,7 +14525,7 @@
       <c r="E223" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F223">
+      <c r="F223" s="72">
         <v>4993</v>
       </c>
       <c r="G223" t="s">
@@ -14522,7 +14551,7 @@
       <c r="E224" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F224">
+      <c r="F224" s="72">
         <v>5871</v>
       </c>
       <c r="G224" t="s">
@@ -14548,7 +14577,7 @@
       <c r="E225" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F225">
+      <c r="F225" s="72">
         <v>6155</v>
       </c>
       <c r="G225" t="s">
@@ -14690,7 +14719,7 @@
       <c r="E230" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F230">
+      <c r="F230" s="72">
         <v>11229</v>
       </c>
       <c r="G230" t="s">
@@ -14716,7 +14745,7 @@
       <c r="E231" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F231">
+      <c r="F231" s="72">
         <v>10472</v>
       </c>
       <c r="G231" t="s">
@@ -14742,7 +14771,7 @@
       <c r="E232" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F232">
+      <c r="F232" s="72">
         <v>9351</v>
       </c>
       <c r="G232" t="s">
@@ -14768,7 +14797,7 @@
       <c r="E233" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F233">
+      <c r="F233" s="72">
         <v>11030</v>
       </c>
       <c r="G233" t="s">
@@ -14794,7 +14823,7 @@
       <c r="E234" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F234">
+      <c r="F234" s="72">
         <v>10210</v>
       </c>
       <c r="G234" t="s">
@@ -14820,7 +14849,7 @@
       <c r="E235" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F235">
+      <c r="F235" s="72">
         <v>37798</v>
       </c>
       <c r="G235" t="s">
@@ -14846,7 +14875,7 @@
       <c r="E236" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F236">
+      <c r="F236" s="72">
         <v>34643</v>
       </c>
       <c r="G236" t="s">
@@ -14860,10 +14889,10 @@
       <c r="A237" t="s">
         <v>87</v>
       </c>
-      <c r="B237" s="81">
+      <c r="B237" s="80">
         <v>1978</v>
       </c>
-      <c r="C237" s="80" t="s">
+      <c r="C237" s="79" t="s">
         <v>164</v>
       </c>
       <c r="D237" t="s">
@@ -14938,10 +14967,10 @@
       <c r="A240" t="s">
         <v>87</v>
       </c>
-      <c r="B240" s="81">
+      <c r="B240" s="80">
         <v>1989</v>
       </c>
-      <c r="C240" s="80" t="s">
+      <c r="C240" s="79" t="s">
         <v>164</v>
       </c>
       <c r="D240" t="s">
@@ -14990,10 +15019,10 @@
       <c r="A242" t="s">
         <v>87</v>
       </c>
-      <c r="B242" s="81">
+      <c r="B242" s="80">
         <v>1994</v>
       </c>
-      <c r="C242" s="80" t="s">
+      <c r="C242" s="79" t="s">
         <v>164</v>
       </c>
       <c r="D242" t="s">
@@ -15792,16 +15821,16 @@
         <v>1995</v>
       </c>
       <c r="C272" s="63" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D272" s="62" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E272" s="59" t="s">
         <v>70</v>
       </c>
       <c r="F272" s="72">
-        <v>6797</v>
+        <v>26435</v>
       </c>
       <c r="G272" t="s">
         <v>180</v>
@@ -16061,7 +16090,7 @@
       <c r="E281" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F281">
+      <c r="F281" s="72">
         <v>28041</v>
       </c>
       <c r="G281" t="s">
@@ -16087,7 +16116,7 @@
       <c r="E282" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F282">
+      <c r="F282" s="72">
         <v>28029</v>
       </c>
       <c r="G282" t="s">
@@ -16139,7 +16168,7 @@
       <c r="E284" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F284">
+      <c r="F284" s="72">
         <v>24977</v>
       </c>
       <c r="G284" t="s">
@@ -16165,7 +16194,7 @@
       <c r="E285" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F285">
+      <c r="F285" s="72">
         <v>25088</v>
       </c>
       <c r="G285" t="s">
@@ -16191,7 +16220,7 @@
       <c r="E286" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F286">
+      <c r="F286" s="72">
         <v>25200</v>
       </c>
       <c r="G286" t="s">
@@ -16217,7 +16246,7 @@
       <c r="E287" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F287">
+      <c r="F287" s="72">
         <v>25350</v>
       </c>
       <c r="G287" t="s">
@@ -16243,7 +16272,7 @@
       <c r="E288" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F288">
+      <c r="F288" s="72">
         <v>20759</v>
       </c>
       <c r="G288" t="s">
@@ -16269,7 +16298,7 @@
       <c r="E289" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F289">
+      <c r="F289" s="72">
         <v>20196</v>
       </c>
       <c r="G289" t="s">
@@ -16295,7 +16324,7 @@
       <c r="E290" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F290">
+      <c r="F290" s="72">
         <v>20137</v>
       </c>
       <c r="G290" t="s">
@@ -16321,7 +16350,7 @@
       <c r="E291" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F291">
+      <c r="F291" s="72">
         <v>19535</v>
       </c>
       <c r="G291" t="s">
@@ -16347,7 +16376,7 @@
       <c r="E292" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F292">
+      <c r="F292" s="72">
         <v>19322</v>
       </c>
       <c r="G292" t="s">
@@ -16373,7 +16402,7 @@
       <c r="E293" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F293">
+      <c r="F293" s="72">
         <v>19380</v>
       </c>
       <c r="G293" t="s">
@@ -16399,7 +16428,7 @@
       <c r="E294" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F294">
+      <c r="F294" s="72">
         <v>19105</v>
       </c>
       <c r="G294" t="s">
@@ -16425,7 +16454,7 @@
       <c r="E295" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F295">
+      <c r="F295" s="72">
         <v>19169</v>
       </c>
       <c r="G295" t="s">
@@ -16451,7 +16480,7 @@
       <c r="E296" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F296">
+      <c r="F296" s="72">
         <v>19210</v>
       </c>
       <c r="G296" t="s">
@@ -16477,7 +16506,7 @@
       <c r="E297" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F297">
+      <c r="F297" s="72">
         <v>10007</v>
       </c>
       <c r="G297" t="s">
@@ -16503,7 +16532,7 @@
       <c r="E298" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F298">
+      <c r="F298" s="72">
         <v>4166</v>
       </c>
       <c r="G298" t="s">
@@ -16529,7 +16558,7 @@
       <c r="E299" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F299">
+      <c r="F299" s="72">
         <v>5669</v>
       </c>
       <c r="G299" t="s">
@@ -16555,7 +16584,7 @@
       <c r="E300" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F300">
+      <c r="F300" s="72">
         <v>2760</v>
       </c>
       <c r="G300" t="s">
@@ -16581,7 +16610,7 @@
       <c r="E301" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F301">
+      <c r="F301" s="72">
         <v>2877</v>
       </c>
       <c r="G301" t="s">
@@ -16607,7 +16636,7 @@
       <c r="E302" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F302">
+      <c r="F302" s="72">
         <v>2827</v>
       </c>
       <c r="G302" t="s">
@@ -16633,7 +16662,7 @@
       <c r="E303" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F303">
+      <c r="F303" s="72">
         <v>2824</v>
       </c>
       <c r="G303" t="s">
@@ -16659,7 +16688,7 @@
       <c r="E304" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F304">
+      <c r="F304" s="72">
         <v>2783</v>
       </c>
       <c r="G304" t="s">
@@ -16685,7 +16714,7 @@
       <c r="E305" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F305">
+      <c r="F305" s="72">
         <v>2768</v>
       </c>
       <c r="G305" t="s">
@@ -16711,7 +16740,7 @@
       <c r="E306" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F306">
+      <c r="F306" s="72">
         <v>2170</v>
       </c>
       <c r="G306" t="s">
@@ -16737,7 +16766,7 @@
       <c r="E307" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F307">
+      <c r="F307" s="72">
         <v>2742</v>
       </c>
       <c r="G307" t="s">
@@ -16763,7 +16792,7 @@
       <c r="E308" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F308">
+      <c r="F308" s="72">
         <v>3243</v>
       </c>
       <c r="G308" t="s">
@@ -16847,7 +16876,7 @@
       <c r="E311" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F311">
+      <c r="F311" s="72">
         <v>5568</v>
       </c>
       <c r="G311" t="s">
@@ -16873,7 +16902,7 @@
       <c r="E312" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F312">
+      <c r="F312" s="72">
         <v>6504</v>
       </c>
       <c r="G312" t="s">
@@ -16899,7 +16928,7 @@
       <c r="E313" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F313">
+      <c r="F313" s="72">
         <v>6029</v>
       </c>
       <c r="G313" t="s">
@@ -16925,7 +16954,7 @@
       <c r="E314" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F314">
+      <c r="F314" s="72">
         <v>8620</v>
       </c>
       <c r="G314" t="s">
@@ -16951,7 +16980,7 @@
       <c r="E315" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F315">
+      <c r="F315" s="72">
         <v>22743</v>
       </c>
       <c r="G315" t="s">
@@ -16977,7 +17006,7 @@
       <c r="E316" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F316">
+      <c r="F316" s="72">
         <v>13686</v>
       </c>
       <c r="G316" t="s">
@@ -17003,7 +17032,7 @@
       <c r="E317" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F317">
+      <c r="F317" s="72">
         <v>13482</v>
       </c>
       <c r="G317" t="s">
@@ -17029,7 +17058,7 @@
       <c r="E318" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F318">
+      <c r="F318" s="72">
         <v>11536</v>
       </c>
       <c r="G318" t="s">
@@ -17113,7 +17142,7 @@
       <c r="E321" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F321" s="79">
+      <c r="F321" s="72">
         <v>2013</v>
       </c>
       <c r="G321" s="62" t="s">
@@ -17142,7 +17171,7 @@
       <c r="E322" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F322">
+      <c r="F322" s="72">
         <v>2058</v>
       </c>
       <c r="G322" t="s">
@@ -17168,7 +17197,7 @@
       <c r="E323" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F323">
+      <c r="F323" s="72">
         <v>2024</v>
       </c>
       <c r="G323" t="s">
@@ -17194,7 +17223,7 @@
       <c r="E324" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F324">
+      <c r="F324" s="72">
         <v>2048</v>
       </c>
       <c r="G324" t="s">
@@ -17220,7 +17249,7 @@
       <c r="E325" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F325">
+      <c r="F325" s="72">
         <v>2061</v>
       </c>
       <c r="G325" t="s">
@@ -17246,7 +17275,7 @@
       <c r="E326" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F326">
+      <c r="F326" s="72">
         <v>2772</v>
       </c>
       <c r="G326" t="s">
@@ -17272,7 +17301,7 @@
       <c r="E327" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F327">
+      <c r="F327" s="72">
         <v>41554</v>
       </c>
       <c r="G327" t="s">
@@ -17298,7 +17327,7 @@
       <c r="E328" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F328">
+      <c r="F328" s="72">
         <v>42152</v>
       </c>
       <c r="G328" t="s">
@@ -17469,7 +17498,7 @@
       <c r="E334" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F334">
+      <c r="F334" s="72">
         <v>3090</v>
       </c>
       <c r="G334" t="s">
@@ -17498,7 +17527,7 @@
       <c r="E335" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F335">
+      <c r="F335" s="72">
         <v>5477</v>
       </c>
       <c r="G335" t="s">
@@ -17527,7 +17556,7 @@
       <c r="E336" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F336">
+      <c r="F336" s="72">
         <v>6085</v>
       </c>
       <c r="G336" t="s">
@@ -17556,7 +17585,7 @@
       <c r="E337" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F337">
+      <c r="F337" s="72">
         <v>5836</v>
       </c>
       <c r="G337" t="s">
@@ -17585,7 +17614,7 @@
       <c r="E338" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F338">
+      <c r="F338" s="72">
         <v>5608</v>
       </c>
       <c r="G338" t="s">
@@ -17614,7 +17643,7 @@
       <c r="E339" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F339">
+      <c r="F339" s="72">
         <v>5247</v>
       </c>
       <c r="G339" t="s">
@@ -17643,7 +17672,7 @@
       <c r="E340" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F340">
+      <c r="F340" s="72">
         <v>5183</v>
       </c>
       <c r="G340" t="s">
@@ -17672,7 +17701,7 @@
       <c r="E341" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F341">
+      <c r="F341" s="72">
         <v>4642</v>
       </c>
       <c r="G341" t="s">
@@ -17701,7 +17730,7 @@
       <c r="E342" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F342">
+      <c r="F342" s="72">
         <v>4333</v>
       </c>
       <c r="G342" t="s">
@@ -17730,7 +17759,7 @@
       <c r="E343" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F343">
+      <c r="F343" s="72">
         <v>4592</v>
       </c>
       <c r="G343" t="s">
@@ -17759,7 +17788,7 @@
       <c r="E344" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F344">
+      <c r="F344" s="72">
         <v>4922</v>
       </c>
       <c r="G344" t="s">
@@ -17788,7 +17817,7 @@
       <c r="E345" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F345">
+      <c r="F345" s="72">
         <v>5486</v>
       </c>
       <c r="G345" t="s">
@@ -17817,7 +17846,7 @@
       <c r="E346" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F346">
+      <c r="F346" s="72">
         <v>5452</v>
       </c>
       <c r="G346" t="s">
@@ -17846,7 +17875,7 @@
       <c r="E347" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F347">
+      <c r="F347" s="72">
         <v>5418</v>
       </c>
       <c r="G347" t="s">
@@ -17875,7 +17904,7 @@
       <c r="E348" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F348">
+      <c r="F348" s="72">
         <v>5029</v>
       </c>
       <c r="G348" t="s">
@@ -17904,7 +17933,7 @@
       <c r="E349" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F349">
+      <c r="F349" s="72">
         <v>4382</v>
       </c>
       <c r="G349" t="s">
@@ -17933,7 +17962,7 @@
       <c r="E350" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F350">
+      <c r="F350" s="72">
         <v>4183</v>
       </c>
       <c r="G350" t="s">
@@ -17962,7 +17991,7 @@
       <c r="E351" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F351">
+      <c r="F351" s="72">
         <v>2928</v>
       </c>
       <c r="G351" t="s">
@@ -17988,7 +18017,7 @@
       <c r="E352" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F352">
+      <c r="F352" s="72">
         <v>2887</v>
       </c>
       <c r="G352" t="s">
@@ -18014,7 +18043,7 @@
       <c r="E353" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F353">
+      <c r="F353" s="72">
         <v>3018</v>
       </c>
       <c r="G353" t="s">
@@ -18040,7 +18069,7 @@
       <c r="E354" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F354">
+      <c r="F354" s="72">
         <v>2271</v>
       </c>
       <c r="G354" t="s">
@@ -18066,7 +18095,7 @@
       <c r="E355" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F355">
+      <c r="F355" s="72">
         <v>5000</v>
       </c>
       <c r="G355" t="s">
@@ -18092,7 +18121,7 @@
       <c r="E356" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F356">
+      <c r="F356" s="72">
         <v>5212</v>
       </c>
       <c r="G356" t="s">
@@ -18118,7 +18147,7 @@
       <c r="E357" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F357">
+      <c r="F357" s="72">
         <v>5230</v>
       </c>
       <c r="G357" t="s">
@@ -18144,7 +18173,7 @@
       <c r="E358" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F358">
+      <c r="F358" s="72">
         <v>5787</v>
       </c>
       <c r="G358" t="s">
@@ -18170,7 +18199,7 @@
       <c r="E359" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F359">
+      <c r="F359" s="72">
         <v>6227</v>
       </c>
       <c r="G359" t="s">
@@ -18196,7 +18225,7 @@
       <c r="E360" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F360">
+      <c r="F360" s="72">
         <v>6218</v>
       </c>
       <c r="G360" t="s">
@@ -18222,7 +18251,7 @@
       <c r="E361" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F361">
+      <c r="F361" s="72">
         <v>6132</v>
       </c>
       <c r="G361" t="s">
@@ -18248,7 +18277,7 @@
       <c r="E362" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F362">
+      <c r="F362" s="72">
         <v>6272</v>
       </c>
       <c r="G362" t="s">
@@ -18274,7 +18303,7 @@
       <c r="E363" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F363">
+      <c r="F363" s="72">
         <v>6259</v>
       </c>
       <c r="G363" t="s">
@@ -18300,7 +18329,7 @@
       <c r="E364" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F364">
+      <c r="F364" s="72">
         <v>6173</v>
       </c>
       <c r="G364" t="s">
@@ -18326,7 +18355,7 @@
       <c r="E365" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F365">
+      <c r="F365" s="72">
         <v>5971</v>
       </c>
       <c r="G365" t="s">
@@ -18352,7 +18381,7 @@
       <c r="E366" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F366">
+      <c r="F366" s="72">
         <v>6270</v>
       </c>
       <c r="G366" t="s">
@@ -18378,7 +18407,7 @@
       <c r="E367" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F367">
+      <c r="F367" s="72">
         <v>6168</v>
       </c>
       <c r="G367" t="s">
@@ -18404,7 +18433,7 @@
       <c r="E368" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F368">
+      <c r="F368" s="72">
         <v>6051</v>
       </c>
       <c r="G368" t="s">
@@ -18430,7 +18459,7 @@
       <c r="E369" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F369">
+      <c r="F369" s="72">
         <v>8742</v>
       </c>
       <c r="G369" t="s">
@@ -18456,7 +18485,7 @@
       <c r="E370" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F370">
+      <c r="F370" s="72">
         <v>9507</v>
       </c>
       <c r="G370" t="s">
@@ -18482,7 +18511,7 @@
       <c r="E371" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F371">
+      <c r="F371" s="72">
         <v>8465</v>
       </c>
       <c r="G371" t="s">
@@ -18508,7 +18537,7 @@
       <c r="E372" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F372">
+      <c r="F372" s="72">
         <v>8550</v>
       </c>
       <c r="G372" t="s">
@@ -18534,7 +18563,7 @@
       <c r="E373" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F373">
+      <c r="F373" s="72">
         <v>8903</v>
       </c>
       <c r="G373" t="s">
@@ -18560,7 +18589,7 @@
       <c r="E374" s="77" t="s">
         <v>343</v>
       </c>
-      <c r="F374">
+      <c r="F374" s="72">
         <v>9017</v>
       </c>
       <c r="G374" t="s">
@@ -18586,7 +18615,7 @@
       <c r="E375" s="77" t="s">
         <v>179</v>
       </c>
-      <c r="F375">
+      <c r="F375" s="72">
         <v>8792</v>
       </c>
       <c r="G375" t="s">
@@ -18612,7 +18641,7 @@
       <c r="E376" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F376">
+      <c r="F376" s="72">
         <v>8022</v>
       </c>
       <c r="G376" t="s">
@@ -18641,7 +18670,7 @@
       <c r="E377" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F377">
+      <c r="F377" s="72">
         <v>8027</v>
       </c>
       <c r="G377" t="s">
@@ -18670,7 +18699,7 @@
       <c r="E378" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F378">
+      <c r="F378" s="72">
         <v>8274</v>
       </c>
       <c r="G378" t="s">
@@ -18699,7 +18728,7 @@
       <c r="E379" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F379">
+      <c r="F379" s="72">
         <v>8188</v>
       </c>
       <c r="G379" t="s">
@@ -18728,7 +18757,7 @@
       <c r="E380" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F380">
+      <c r="F380" s="72">
         <v>8089</v>
       </c>
       <c r="G380" t="s">
@@ -18757,7 +18786,7 @@
       <c r="E381" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F381">
+      <c r="F381" s="72">
         <v>8135</v>
       </c>
       <c r="G381" t="s">
@@ -18786,7 +18815,7 @@
       <c r="E382" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F382">
+      <c r="F382" s="72">
         <v>7147</v>
       </c>
       <c r="G382" t="s">
@@ -18815,7 +18844,7 @@
       <c r="E383" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F383">
+      <c r="F383" s="72">
         <v>8001</v>
       </c>
       <c r="G383" t="s">
@@ -18844,7 +18873,7 @@
       <c r="E384" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F384">
+      <c r="F384" s="72">
         <v>8012</v>
       </c>
       <c r="G384" t="s">
@@ -18873,7 +18902,7 @@
       <c r="E385" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F385">
+      <c r="F385" s="72">
         <v>7977</v>
       </c>
       <c r="G385" t="s">
@@ -18902,7 +18931,7 @@
       <c r="E386" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F386">
+      <c r="F386" s="72">
         <v>7951</v>
       </c>
       <c r="G386" t="s">
@@ -18931,7 +18960,7 @@
       <c r="E387" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F387">
+      <c r="F387" s="72">
         <v>8156</v>
       </c>
       <c r="G387" t="s">
@@ -18960,7 +18989,7 @@
       <c r="E388" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F388">
+      <c r="F388" s="72">
         <v>7421</v>
       </c>
       <c r="G388" t="s">
@@ -18989,7 +19018,7 @@
       <c r="E389" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F389">
+      <c r="F389" s="72">
         <v>4022</v>
       </c>
       <c r="G389" t="s">
@@ -19018,7 +19047,7 @@
       <c r="E390" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F390">
+      <c r="F390" s="72">
         <v>3160</v>
       </c>
       <c r="G390" t="s">
@@ -19047,7 +19076,7 @@
       <c r="E391" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F391">
+      <c r="F391" s="72">
         <v>2358</v>
       </c>
       <c r="G391" t="s">
@@ -19076,7 +19105,7 @@
       <c r="E392" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F392">
+      <c r="F392" s="72">
         <v>15532</v>
       </c>
       <c r="G392" t="s">
@@ -19102,7 +19131,7 @@
       <c r="E393" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F393">
+      <c r="F393" s="72">
         <v>13655</v>
       </c>
       <c r="G393" t="s">
@@ -19128,7 +19157,7 @@
       <c r="E394" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F394">
+      <c r="F394" s="72">
         <v>13317</v>
       </c>
       <c r="G394" t="s">
@@ -19154,7 +19183,7 @@
       <c r="E395" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F395">
+      <c r="F395" s="72">
         <v>13075</v>
       </c>
       <c r="G395" t="s">
@@ -19180,7 +19209,7 @@
       <c r="E396" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F396">
+      <c r="F396" s="72">
         <v>12377</v>
       </c>
       <c r="G396" t="s">
@@ -19206,7 +19235,7 @@
       <c r="E397" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F397">
+      <c r="F397" s="72">
         <v>11442</v>
       </c>
       <c r="G397" t="s">
@@ -19232,7 +19261,7 @@
       <c r="E398" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F398">
+      <c r="F398" s="72">
         <v>5314</v>
       </c>
       <c r="G398" t="s">
@@ -19258,7 +19287,7 @@
       <c r="E399" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F399">
+      <c r="F399" s="72">
         <v>5200</v>
       </c>
       <c r="G399" t="s">
@@ -19284,7 +19313,7 @@
       <c r="E400" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F400">
+      <c r="F400" s="72">
         <v>5394</v>
       </c>
       <c r="G400" t="s">
@@ -19310,7 +19339,7 @@
       <c r="E401" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F401">
+      <c r="F401" s="72">
         <v>5142</v>
       </c>
       <c r="G401" t="s">
@@ -19336,7 +19365,7 @@
       <c r="E402" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F402">
+      <c r="F402" s="72">
         <v>5194</v>
       </c>
       <c r="G402" t="s">
@@ -19362,7 +19391,7 @@
       <c r="E403" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F403">
+      <c r="F403" s="72">
         <v>4849</v>
       </c>
       <c r="G403" t="s">
@@ -19388,7 +19417,7 @@
       <c r="E404" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F404">
+      <c r="F404" s="72">
         <v>4808</v>
       </c>
       <c r="G404" t="s">
@@ -19414,7 +19443,7 @@
       <c r="E405" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F405">
+      <c r="F405" s="72">
         <v>4944</v>
       </c>
       <c r="G405" t="s">
@@ -19440,7 +19469,7 @@
       <c r="E406" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F406">
+      <c r="F406" s="72">
         <v>4905</v>
       </c>
       <c r="G406" t="s">
@@ -19466,7 +19495,7 @@
       <c r="E407" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F407">
+      <c r="F407" s="72">
         <v>5131</v>
       </c>
       <c r="G407" t="s">
@@ -19637,7 +19666,7 @@
       <c r="E413" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F413">
+      <c r="F413" s="72">
         <v>3622</v>
       </c>
       <c r="G413" t="s">
@@ -19663,7 +19692,7 @@
       <c r="E414" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F414">
+      <c r="F414" s="72">
         <v>3779</v>
       </c>
       <c r="G414" t="s">
@@ -19689,7 +19718,7 @@
       <c r="E415" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F415">
+      <c r="F415" s="72">
         <v>5464</v>
       </c>
       <c r="G415" t="s">
@@ -19715,7 +19744,7 @@
       <c r="E416" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F416">
+      <c r="F416" s="72">
         <v>3879</v>
       </c>
       <c r="G416" t="s">
@@ -19741,6 +19770,7 @@
       <c r="E417" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F417" s="72"/>
       <c r="G417" t="s">
         <v>174</v>
       </c>
@@ -19764,6 +19794,7 @@
       <c r="E418" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F418" s="72"/>
       <c r="G418" t="s">
         <v>174</v>
       </c>
@@ -19787,6 +19818,7 @@
       <c r="E419" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F419" s="72"/>
       <c r="G419" t="s">
         <v>174</v>
       </c>
@@ -19810,6 +19842,7 @@
       <c r="E420" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F420" s="72"/>
       <c r="G420" t="s">
         <v>174</v>
       </c>
@@ -19833,6 +19866,7 @@
       <c r="E421" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F421" s="72"/>
       <c r="G421" t="s">
         <v>174</v>
       </c>
@@ -19856,7 +19890,7 @@
       <c r="E422" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F422">
+      <c r="F422" s="72">
         <v>6893</v>
       </c>
       <c r="G422" t="s">
@@ -19885,6 +19919,7 @@
       <c r="E423" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F423" s="72"/>
       <c r="G423" t="s">
         <v>298</v>
       </c>
@@ -19911,6 +19946,7 @@
       <c r="E424" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F424" s="72"/>
       <c r="G424" t="s">
         <v>298</v>
       </c>
@@ -19937,6 +19973,7 @@
       <c r="E425" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F425" s="72"/>
       <c r="G425" t="s">
         <v>298</v>
       </c>
@@ -19963,6 +20000,7 @@
       <c r="E426" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F426" s="72"/>
       <c r="G426" t="s">
         <v>298</v>
       </c>
@@ -19989,6 +20027,7 @@
       <c r="E427" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F427" s="72"/>
       <c r="G427" t="s">
         <v>298</v>
       </c>
@@ -20015,6 +20054,7 @@
       <c r="E428" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F428" s="72"/>
       <c r="G428" t="s">
         <v>298</v>
       </c>
@@ -20041,6 +20081,7 @@
       <c r="E429" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F429" s="72"/>
       <c r="G429" t="s">
         <v>298</v>
       </c>
@@ -20056,7 +20097,7 @@
         <v>346</v>
       </c>
       <c r="B430" s="1">
-        <v>2010</v>
+        <v>2020</v>
       </c>
       <c r="C430" t="s">
         <v>347</v>
@@ -20067,6 +20108,7 @@
       <c r="E430" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F430" s="72"/>
       <c r="G430" t="s">
         <v>298</v>
       </c>
@@ -20093,7 +20135,7 @@
       <c r="E431" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F431">
+      <c r="F431" s="72">
         <v>4735</v>
       </c>
       <c r="G431" t="s">
@@ -20119,7 +20161,7 @@
       <c r="E432" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F432">
+      <c r="F432" s="72">
         <v>11531</v>
       </c>
       <c r="G432" t="s">
@@ -20145,7 +20187,7 @@
       <c r="E433" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F433">
+      <c r="F433" s="72">
         <v>10530</v>
       </c>
       <c r="G433" t="s">
@@ -20171,7 +20213,7 @@
       <c r="E434" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F434">
+      <c r="F434" s="72">
         <v>12815</v>
       </c>
       <c r="G434" t="s">
@@ -20197,7 +20239,7 @@
       <c r="E435" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F435">
+      <c r="F435" s="72">
         <v>14042</v>
       </c>
       <c r="G435" t="s">
@@ -20223,7 +20265,7 @@
       <c r="E436" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F436">
+      <c r="F436" s="72">
         <v>10952</v>
       </c>
       <c r="G436" t="s">
@@ -20249,7 +20291,7 @@
       <c r="E437" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F437">
+      <c r="F437" s="72">
         <v>10108</v>
       </c>
       <c r="G437" t="s">
@@ -20275,7 +20317,7 @@
       <c r="E438" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F438">
+      <c r="F438" s="72">
         <v>17167</v>
       </c>
       <c r="G438" t="s">
@@ -20301,7 +20343,7 @@
       <c r="E439" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F439">
+      <c r="F439" s="72">
         <v>22595</v>
       </c>
       <c r="G439" t="s">
@@ -20327,7 +20369,7 @@
       <c r="E440" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F440">
+      <c r="F440" s="72">
         <v>23174</v>
       </c>
       <c r="G440" t="s">
@@ -20353,7 +20395,7 @@
       <c r="E441" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F441">
+      <c r="F441" s="72">
         <v>20875</v>
       </c>
       <c r="G441" t="s">
@@ -20379,7 +20421,7 @@
       <c r="E442" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F442">
+      <c r="F442" s="72">
         <v>10337</v>
       </c>
       <c r="G442" t="s">
@@ -20405,7 +20447,7 @@
       <c r="E443" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F443">
+      <c r="F443" s="72">
         <v>27655</v>
       </c>
       <c r="G443" t="s">
@@ -20431,7 +20473,7 @@
       <c r="E444" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F444">
+      <c r="F444" s="72">
         <v>9002</v>
       </c>
       <c r="G444" t="s">
@@ -20457,7 +20499,7 @@
       <c r="E445" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F445">
+      <c r="F445" s="72">
         <v>19479</v>
       </c>
       <c r="G445" t="s">
@@ -20483,7 +20525,7 @@
       <c r="E446" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F446">
+      <c r="F446" s="72">
         <v>70311</v>
       </c>
       <c r="G446" t="s">
@@ -20509,7 +20551,7 @@
       <c r="E447" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F447">
+      <c r="F447" s="72">
         <v>74647</v>
       </c>
       <c r="G447" t="s">
@@ -21057,7 +21099,7 @@
       <c r="E466" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F466">
+      <c r="F466" s="72">
         <v>13131</v>
       </c>
       <c r="G466" t="s">
@@ -21083,7 +21125,7 @@
       <c r="E467" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F467">
+      <c r="F467" s="72">
         <v>217884</v>
       </c>
       <c r="G467" t="s">
@@ -21109,7 +21151,7 @@
       <c r="E468" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F468">
+      <c r="F468" s="72">
         <v>228200</v>
       </c>
       <c r="G468" t="s">
@@ -21135,7 +21177,7 @@
       <c r="E469" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F469">
+      <c r="F469" s="72">
         <v>235732</v>
       </c>
       <c r="G469" t="s">
@@ -21161,7 +21203,7 @@
       <c r="E470" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F470">
+      <c r="F470" s="72">
         <v>243915</v>
       </c>
       <c r="G470" t="s">
@@ -21187,7 +21229,7 @@
       <c r="E471" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F471">
+      <c r="F471" s="72">
         <v>257116</v>
       </c>
       <c r="G471" t="s">
@@ -21213,7 +21255,7 @@
       <c r="E472" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F472">
+      <c r="F472" s="72">
         <v>261320</v>
       </c>
       <c r="G472" t="s">
@@ -21239,7 +21281,7 @@
       <c r="E473" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F473">
+      <c r="F473" s="72">
         <v>3736</v>
       </c>
       <c r="G473" t="s">
@@ -21265,7 +21307,7 @@
       <c r="E474" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F474">
+      <c r="F474" s="72">
         <v>13091</v>
       </c>
       <c r="G474" t="s">
@@ -21291,7 +21333,7 @@
       <c r="E475" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F475">
+      <c r="F475" s="72">
         <v>13391</v>
       </c>
       <c r="G475" t="s">
@@ -21317,7 +21359,7 @@
       <c r="E476" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F476">
+      <c r="F476" s="72">
         <v>11905</v>
       </c>
       <c r="G476" t="s">
@@ -21346,7 +21388,7 @@
       <c r="E477" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F477">
+      <c r="F477" s="72">
         <v>11610</v>
       </c>
       <c r="G477" t="s">
@@ -21375,7 +21417,7 @@
       <c r="E478" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F478">
+      <c r="F478" s="72">
         <v>19502</v>
       </c>
       <c r="G478" t="s">
@@ -21401,6 +21443,7 @@
       <c r="E479" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F479" s="72"/>
       <c r="G479" t="s">
         <v>309</v>
       </c>
@@ -21424,6 +21467,7 @@
       <c r="E480" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F480" s="72"/>
       <c r="G480" t="s">
         <v>309</v>
       </c>
@@ -21447,7 +21491,7 @@
       <c r="E481" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F481">
+      <c r="F481" s="72">
         <v>22204</v>
       </c>
       <c r="G481" t="s">
@@ -21473,6 +21517,7 @@
       <c r="E482" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F482" s="72"/>
       <c r="G482" t="s">
         <v>309</v>
       </c>
@@ -21496,6 +21541,7 @@
       <c r="E483" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F483" s="72"/>
       <c r="G483" t="s">
         <v>309</v>
       </c>
@@ -21519,7 +21565,7 @@
       <c r="E484" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F484">
+      <c r="F484" s="72">
         <v>21496</v>
       </c>
       <c r="G484" t="s">
@@ -21546,6 +21592,7 @@
       <c r="E485" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F485" s="72"/>
       <c r="G485" t="s">
         <v>309</v>
       </c>
@@ -21570,6 +21617,7 @@
       <c r="E486" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F486" s="72"/>
       <c r="G486" t="s">
         <v>309</v>
       </c>
@@ -21594,7 +21642,7 @@
       <c r="E487" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F487">
+      <c r="F487" s="72">
         <v>30453</v>
       </c>
       <c r="G487" t="s">
@@ -21620,6 +21668,7 @@
       <c r="E488" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F488" s="72"/>
       <c r="G488" t="s">
         <v>309</v>
       </c>
@@ -21643,6 +21692,7 @@
       <c r="E489" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F489" s="72"/>
       <c r="G489" t="s">
         <v>309</v>
       </c>
@@ -21666,7 +21716,7 @@
       <c r="E490" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F490">
+      <c r="F490" s="72">
         <v>35785</v>
       </c>
       <c r="G490" t="s">
@@ -21692,6 +21742,7 @@
       <c r="E491" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F491" s="72"/>
       <c r="G491" t="s">
         <v>309</v>
       </c>
@@ -21715,6 +21766,7 @@
       <c r="E492" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F492" s="72"/>
       <c r="G492" t="s">
         <v>309</v>
       </c>
@@ -21738,6 +21790,7 @@
       <c r="E493" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F493" s="72"/>
       <c r="G493" t="s">
         <v>309</v>
       </c>
@@ -21877,7 +21930,7 @@
       <c r="E498" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F498">
+      <c r="F498" s="72">
         <v>32214</v>
       </c>
       <c r="G498" t="s">
@@ -21955,7 +22008,7 @@
       <c r="E501" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F501">
+      <c r="F501" s="72">
         <v>37366</v>
       </c>
       <c r="G501" t="s">
@@ -22033,7 +22086,7 @@
       <c r="E504" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F504">
+      <c r="F504" s="72">
         <v>37412</v>
       </c>
       <c r="G504" t="s">
@@ -22111,7 +22164,7 @@
       <c r="E507" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F507">
+      <c r="F507" s="72">
         <v>37181</v>
       </c>
       <c r="G507" t="s">
@@ -22189,7 +22242,7 @@
       <c r="E510" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F510">
+      <c r="F510" s="72">
         <v>36886</v>
       </c>
       <c r="G510" t="s">
@@ -22215,7 +22268,7 @@
       <c r="E511" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F511">
+      <c r="F511" s="72">
         <v>36655</v>
       </c>
       <c r="G511" t="s">
@@ -22241,7 +22294,7 @@
       <c r="E512" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F512">
+      <c r="F512" s="72">
         <v>36166</v>
       </c>
       <c r="G512" t="s">
@@ -22267,7 +22320,7 @@
       <c r="E513" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F513">
+      <c r="F513" s="72">
         <v>35923</v>
       </c>
       <c r="G513" t="s">
@@ -22293,7 +22346,7 @@
       <c r="E514" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F514">
+      <c r="F514" s="72">
         <v>33529</v>
       </c>
       <c r="G514" t="s">
@@ -22319,7 +22372,7 @@
       <c r="E515" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F515">
+      <c r="F515" s="72">
         <v>4353</v>
       </c>
       <c r="G515" t="s">
@@ -22345,7 +22398,7 @@
       <c r="E516" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F516">
+      <c r="F516" s="72">
         <v>5101</v>
       </c>
       <c r="G516" t="s">
@@ -22371,7 +22424,7 @@
       <c r="E517" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F517">
+      <c r="F517" s="72">
         <v>8131</v>
       </c>
       <c r="G517" t="s">
@@ -22397,7 +22450,7 @@
       <c r="E518" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F518">
+      <c r="F518" s="72">
         <v>3789</v>
       </c>
       <c r="G518" t="s">
@@ -22423,7 +22476,7 @@
       <c r="E519" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F519">
+      <c r="F519" s="72">
         <v>9591</v>
       </c>
       <c r="G519" t="s">
@@ -22449,7 +22502,7 @@
       <c r="E520" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F520">
+      <c r="F520" s="72">
         <v>7823</v>
       </c>
       <c r="G520" t="s">
@@ -22475,7 +22528,7 @@
       <c r="E521" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F521">
+      <c r="F521" s="72">
         <v>4464</v>
       </c>
       <c r="G521" t="s">
@@ -22501,7 +22554,7 @@
       <c r="E522" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F522">
+      <c r="F522" s="72">
         <v>5292</v>
       </c>
       <c r="G522" t="s">
@@ -22527,7 +22580,7 @@
       <c r="E523" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F523">
+      <c r="F523" s="72">
         <v>4812</v>
       </c>
       <c r="G523" t="s">
@@ -22553,7 +22606,7 @@
       <c r="E524" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F524">
+      <c r="F524" s="72">
         <v>4601</v>
       </c>
       <c r="G524" t="s">
@@ -22579,7 +22632,7 @@
       <c r="E525" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F525">
+      <c r="F525" s="72">
         <v>4439</v>
       </c>
       <c r="G525" t="s">
@@ -22605,7 +22658,7 @@
       <c r="E526" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F526">
+      <c r="F526" s="72">
         <v>5003</v>
       </c>
       <c r="G526" t="s">
@@ -22631,7 +22684,7 @@
       <c r="E527" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F527">
+      <c r="F527" s="72">
         <v>4894</v>
       </c>
       <c r="G527" t="s">
@@ -22657,7 +22710,7 @@
       <c r="E528" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F528">
+      <c r="F528" s="72">
         <v>5288</v>
       </c>
       <c r="G528" t="s">
@@ -22683,7 +22736,7 @@
       <c r="E529" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F529">
+      <c r="F529" s="72">
         <v>5424</v>
       </c>
       <c r="G529" t="s">
@@ -22709,7 +22762,7 @@
       <c r="E530" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F530">
+      <c r="F530" s="72">
         <v>5165</v>
       </c>
       <c r="G530" t="s">
@@ -22735,7 +22788,7 @@
       <c r="E531" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F531">
+      <c r="F531" s="72">
         <v>8229</v>
       </c>
       <c r="G531" t="s">
@@ -22761,7 +22814,7 @@
       <c r="E532" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F532">
+      <c r="F532" s="72">
         <v>10219</v>
       </c>
       <c r="G532" t="s">
@@ -22787,7 +22840,7 @@
       <c r="E533" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F533">
+      <c r="F533" s="72">
         <v>9570</v>
       </c>
       <c r="G533" t="s">
@@ -22813,7 +22866,7 @@
       <c r="E534" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F534">
+      <c r="F534" s="72">
         <v>4999</v>
       </c>
       <c r="G534" t="s">
@@ -22839,7 +22892,7 @@
       <c r="E535" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F535">
+      <c r="F535" s="72">
         <v>5099</v>
       </c>
       <c r="G535" t="s">
@@ -22865,7 +22918,7 @@
       <c r="E536" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F536">
+      <c r="F536" s="72">
         <v>4842</v>
       </c>
       <c r="G536" t="s">
@@ -22949,7 +23002,7 @@
       <c r="E539" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F539">
+      <c r="F539" s="72">
         <v>3319</v>
       </c>
       <c r="G539" t="s">
@@ -22975,7 +23028,7 @@
       <c r="E540" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F540">
+      <c r="F540" s="72">
         <v>3394</v>
       </c>
       <c r="G540" t="s">
@@ -23001,7 +23054,7 @@
       <c r="E541" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F541">
+      <c r="F541" s="72">
         <v>3933</v>
       </c>
       <c r="G541" t="s">
@@ -23027,7 +23080,7 @@
       <c r="E542" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F542">
+      <c r="F542" s="72">
         <v>6323</v>
       </c>
       <c r="G542" t="s">
@@ -23053,7 +23106,7 @@
       <c r="E543" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F543">
+      <c r="F543" s="72">
         <v>9990</v>
       </c>
       <c r="G543" t="s">
@@ -23079,7 +23132,7 @@
       <c r="E544" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F544">
+      <c r="F544" s="72">
         <v>45000</v>
       </c>
       <c r="G544" t="s">
@@ -23105,7 +23158,7 @@
       <c r="E545" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F545">
+      <c r="F545" s="72">
         <v>45000</v>
       </c>
       <c r="G545" t="s">
@@ -23131,7 +23184,7 @@
       <c r="E546" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F546">
+      <c r="F546" s="72">
         <v>60000</v>
       </c>
       <c r="G546" t="s">
@@ -23157,7 +23210,7 @@
       <c r="E547" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F547">
+      <c r="F547" s="72">
         <v>160008</v>
       </c>
       <c r="G547" t="s">
@@ -23183,7 +23236,7 @@
       <c r="E548" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F548">
+      <c r="F548" s="72">
         <v>60000</v>
       </c>
       <c r="G548" t="s">
@@ -23209,7 +23262,7 @@
       <c r="E549" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F549">
+      <c r="F549" s="72">
         <v>60000</v>
       </c>
       <c r="G549" t="s">
@@ -23235,7 +23288,7 @@
       <c r="E550" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F550">
+      <c r="F550" s="72">
         <v>60000</v>
       </c>
       <c r="G550" t="s">
@@ -23261,7 +23314,7 @@
       <c r="E551" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F551">
+      <c r="F551" s="72">
         <v>4560</v>
       </c>
       <c r="G551" t="s">
@@ -23287,7 +23340,7 @@
       <c r="E552" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F552">
+      <c r="F552" s="72">
         <v>4585</v>
       </c>
       <c r="G552" t="s">
@@ -23313,7 +23366,7 @@
       <c r="E553" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F553">
+      <c r="F553" s="72">
         <v>4517</v>
       </c>
       <c r="G553" t="s">
@@ -23339,7 +23392,7 @@
       <c r="E554" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F554">
+      <c r="F554" s="72">
         <v>6457</v>
       </c>
       <c r="G554" t="s">
@@ -23539,7 +23592,7 @@
       <c r="E561" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F561" s="62">
+      <c r="F561" s="72">
         <v>5637</v>
       </c>
       <c r="G561" t="s">
@@ -23565,7 +23618,7 @@
       <c r="E562" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F562" s="62">
+      <c r="F562" s="72">
         <v>5738</v>
       </c>
       <c r="G562" t="s">
@@ -23591,7 +23644,7 @@
       <c r="E563" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F563" s="62">
+      <c r="F563" s="72">
         <v>5602</v>
       </c>
       <c r="G563" t="s">
@@ -23617,7 +23670,7 @@
       <c r="E564" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F564" s="62">
+      <c r="F564" s="72">
         <v>5662</v>
       </c>
       <c r="G564" t="s">
@@ -23643,7 +23696,7 @@
       <c r="E565" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F565" s="62">
+      <c r="F565" s="72">
         <v>5591</v>
       </c>
       <c r="G565" t="s">
@@ -23727,7 +23780,7 @@
       <c r="E568" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F568">
+      <c r="F568" s="72">
         <v>3725</v>
       </c>
       <c r="G568" t="s">
@@ -23753,7 +23806,7 @@
       <c r="E569" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F569">
+      <c r="F569" s="72">
         <v>3697</v>
       </c>
       <c r="G569" t="s">
@@ -23779,7 +23832,7 @@
       <c r="E570" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F570">
+      <c r="F570" s="72">
         <v>3924</v>
       </c>
       <c r="G570" t="s">
@@ -23805,7 +23858,7 @@
       <c r="E571" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F571">
+      <c r="F571" s="72">
         <v>3663</v>
       </c>
       <c r="G571" t="s">
@@ -23831,7 +23884,7 @@
       <c r="E572" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F572">
+      <c r="F572" s="72">
         <v>3750</v>
       </c>
       <c r="G572" t="s">
@@ -23842,16 +23895,16 @@
       </c>
     </row>
     <row r="573" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A573" t="s">
+      <c r="A573" s="81" t="s">
         <v>134</v>
       </c>
-      <c r="B573" s="1">
+      <c r="B573" s="82">
         <v>1967</v>
       </c>
-      <c r="C573" s="63" t="s">
+      <c r="C573" s="83" t="s">
         <v>135</v>
       </c>
-      <c r="D573" s="62" t="s">
+      <c r="D573" s="81" t="s">
         <v>168</v>
       </c>
       <c r="E573" s="59" t="s">
@@ -24060,7 +24113,7 @@
       <c r="E580" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F580">
+      <c r="F580" s="72">
         <v>16268</v>
       </c>
       <c r="G580" t="s">
@@ -24405,7 +24458,7 @@
       <c r="E592" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F592">
+      <c r="F592" s="72">
         <v>18392</v>
       </c>
       <c r="G592" t="s">
@@ -24431,6 +24484,7 @@
       <c r="E593" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F593" s="72"/>
       <c r="G593" t="s">
         <v>320</v>
       </c>
@@ -24454,6 +24508,7 @@
       <c r="E594" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F594" s="72"/>
       <c r="G594" t="s">
         <v>320</v>
       </c>
@@ -24477,7 +24532,7 @@
       <c r="E595" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F595">
+      <c r="F595" s="72">
         <v>49136</v>
       </c>
       <c r="G595" t="s">
@@ -24503,6 +24558,7 @@
       <c r="E596" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F596" s="72"/>
       <c r="G596" t="s">
         <v>320</v>
       </c>
@@ -24526,6 +24582,7 @@
       <c r="E597" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F597" s="72"/>
       <c r="G597" t="s">
         <v>320</v>
       </c>
@@ -24549,7 +24606,7 @@
       <c r="E598" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F598">
+      <c r="F598" s="72">
         <v>46550</v>
       </c>
       <c r="G598" t="s">
@@ -24575,6 +24632,7 @@
       <c r="E599" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F599" s="72"/>
       <c r="G599" t="s">
         <v>320</v>
       </c>
@@ -24598,6 +24656,7 @@
       <c r="E600" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F600" s="72"/>
       <c r="G600" t="s">
         <v>320</v>
       </c>
@@ -24621,7 +24680,7 @@
       <c r="E601" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F601">
+      <c r="F601" s="72">
         <v>46622</v>
       </c>
       <c r="G601" t="s">
@@ -24647,6 +24706,7 @@
       <c r="E602" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F602" s="72"/>
       <c r="G602" t="s">
         <v>320</v>
       </c>
@@ -24670,6 +24730,7 @@
       <c r="E603" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F603" s="72"/>
       <c r="G603" t="s">
         <v>320</v>
       </c>
@@ -24693,7 +24754,7 @@
       <c r="E604" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F604">
+      <c r="F604" s="72">
         <v>45158</v>
       </c>
       <c r="G604" t="s">
@@ -24719,6 +24780,7 @@
       <c r="E605" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F605" s="72"/>
       <c r="G605" t="s">
         <v>320</v>
       </c>
@@ -24742,6 +24804,7 @@
       <c r="E606" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F606" s="72"/>
       <c r="G606" t="s">
         <v>320</v>
       </c>
@@ -24765,6 +24828,7 @@
       <c r="E607" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="F607" s="72"/>
       <c r="G607" t="s">
         <v>320</v>
       </c>
@@ -24817,7 +24881,7 @@
       <c r="E609" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F609">
+      <c r="F609" s="72">
         <v>65238</v>
       </c>
       <c r="G609" t="s">
@@ -24843,7 +24907,7 @@
       <c r="E610" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F610">
+      <c r="F610" s="72">
         <v>65731</v>
       </c>
       <c r="G610" t="s">
@@ -24869,7 +24933,7 @@
       <c r="E611" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F611">
+      <c r="F611" s="72">
         <v>59276</v>
       </c>
       <c r="G611" t="s">
@@ -24895,7 +24959,7 @@
       <c r="E612" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F612">
+      <c r="F612" s="72">
         <v>59211</v>
       </c>
       <c r="G612" t="s">
@@ -24921,7 +24985,7 @@
       <c r="E613" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F613">
+      <c r="F613" s="72">
         <v>59171</v>
       </c>
       <c r="G613" t="s">
@@ -24947,7 +25011,7 @@
       <c r="E614" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F614">
+      <c r="F614" s="72">
         <v>59799</v>
       </c>
       <c r="G614" t="s">
@@ -24973,7 +25037,7 @@
       <c r="E615" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F615">
+      <c r="F615" s="72">
         <v>58914</v>
       </c>
       <c r="G615" t="s">
@@ -24999,7 +25063,7 @@
       <c r="E616" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F616">
+      <c r="F616" s="72">
         <v>58258</v>
       </c>
       <c r="G616" t="s">
@@ -25025,7 +25089,7 @@
       <c r="E617" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F617">
+      <c r="F617" s="72">
         <v>58975</v>
       </c>
       <c r="G617" t="s">
@@ -25051,7 +25115,7 @@
       <c r="E618" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F618">
+      <c r="F618" s="72">
         <v>55335</v>
       </c>
       <c r="G618" t="s">
@@ -25077,7 +25141,7 @@
       <c r="E619" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F619">
+      <c r="F619" s="72">
         <v>59941</v>
       </c>
       <c r="G619" t="s">
@@ -25103,7 +25167,7 @@
       <c r="E620" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F620">
+      <c r="F620" s="72">
         <v>59929</v>
       </c>
       <c r="G620" t="s">
@@ -25129,7 +25193,7 @@
       <c r="E621" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F621">
+      <c r="F621" s="72">
         <v>59219</v>
       </c>
       <c r="G621" t="s">
@@ -25155,7 +25219,7 @@
       <c r="E622" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F622">
+      <c r="F622" s="72">
         <v>58970</v>
       </c>
       <c r="G622" t="s">
@@ -25181,7 +25245,7 @@
       <c r="E623" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F623">
+      <c r="F623" s="72">
         <v>57079</v>
       </c>
       <c r="G623" t="s">
@@ -25207,7 +25271,7 @@
       <c r="E624" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F624">
+      <c r="F624" s="72">
         <v>56941</v>
       </c>
       <c r="G624" t="s">
@@ -25233,7 +25297,7 @@
       <c r="E625" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F625">
+      <c r="F625" s="72">
         <v>49682</v>
       </c>
       <c r="G625" t="s">
@@ -25259,7 +25323,7 @@
       <c r="E626" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F626">
+      <c r="F626" s="72">
         <v>50311</v>
       </c>
       <c r="G626" t="s">
@@ -25285,7 +25349,7 @@
       <c r="E627" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F627">
+      <c r="F627" s="72">
         <v>50348</v>
       </c>
       <c r="G627" t="s">
@@ -25311,7 +25375,7 @@
       <c r="E628" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F628">
+      <c r="F628" s="72">
         <v>50781</v>
       </c>
       <c r="G628" t="s">
@@ -25337,7 +25401,7 @@
       <c r="E629" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F629">
+      <c r="F629" s="72">
         <v>51016</v>
       </c>
       <c r="G629" t="s">
@@ -25363,7 +25427,7 @@
       <c r="E630" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F630">
+      <c r="F630" s="72">
         <v>78054</v>
       </c>
       <c r="G630" t="s">
@@ -25389,7 +25453,7 @@
       <c r="E631" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F631">
+      <c r="F631" s="72">
         <v>78265</v>
       </c>
       <c r="G631" t="s">
@@ -25415,7 +25479,7 @@
       <c r="E632" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F632">
+      <c r="F632" s="72">
         <v>78310</v>
       </c>
       <c r="G632" t="s">
@@ -25441,7 +25505,7 @@
       <c r="E633" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F633">
+      <c r="F633" s="72">
         <v>77149</v>
       </c>
       <c r="G633" t="s">
@@ -25467,7 +25531,7 @@
       <c r="E634" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F634">
+      <c r="F634" s="72">
         <v>76447</v>
       </c>
       <c r="G634" t="s">
@@ -25493,7 +25557,7 @@
       <c r="E635" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F635">
+      <c r="F635" s="72">
         <v>75939</v>
       </c>
       <c r="G635" t="s">
@@ -25519,7 +25583,7 @@
       <c r="E636" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F636">
+      <c r="F636" s="72">
         <v>75477</v>
       </c>
       <c r="G636" t="s">
@@ -25545,7 +25609,7 @@
       <c r="E637" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F637">
+      <c r="F637" s="72">
         <v>75872</v>
       </c>
       <c r="G637" t="s">
@@ -25571,7 +25635,7 @@
       <c r="E638" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F638">
+      <c r="F638" s="72">
         <v>76185</v>
       </c>
       <c r="G638" t="s">
@@ -25597,7 +25661,7 @@
       <c r="E639" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F639">
+      <c r="F639" s="72">
         <v>76260</v>
       </c>
       <c r="G639" t="s">
@@ -25623,7 +25687,7 @@
       <c r="E640" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F640">
+      <c r="F640" s="72">
         <v>75188</v>
       </c>
       <c r="G640" t="s">
@@ -25649,7 +25713,7 @@
       <c r="E641" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F641">
+      <c r="F641" s="72">
         <v>74383</v>
       </c>
       <c r="G641" t="s">
@@ -25675,7 +25739,7 @@
       <c r="E642" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F642">
+      <c r="F642" s="72">
         <v>74821</v>
       </c>
       <c r="G642" t="s">
@@ -25701,7 +25765,7 @@
       <c r="E643" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F643">
+      <c r="F643" s="72">
         <v>51498</v>
       </c>
       <c r="G643" t="s">
@@ -25727,7 +25791,7 @@
       <c r="E644" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F644">
+      <c r="F644" s="72">
         <v>74257</v>
       </c>
       <c r="G644" t="s">
@@ -25753,7 +25817,7 @@
       <c r="E645" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F645">
+      <c r="F645" s="72">
         <v>69484</v>
       </c>
       <c r="G645" t="s">
@@ -25779,7 +25843,7 @@
       <c r="E646" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F646">
+      <c r="F646" s="72">
         <v>69957</v>
       </c>
       <c r="G646" t="s">
@@ -25805,7 +25869,7 @@
       <c r="E647" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F647">
+      <c r="F647" s="72">
         <v>67909</v>
       </c>
       <c r="G647" t="s">
@@ -25831,7 +25895,7 @@
       <c r="E648" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F648">
+      <c r="F648" s="72">
         <v>68345</v>
       </c>
       <c r="G648" t="s">
@@ -25857,7 +25921,7 @@
       <c r="E649" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F649">
+      <c r="F649" s="72">
         <v>60460</v>
       </c>
       <c r="G649" t="s">
@@ -25883,7 +25947,7 @@
       <c r="E650" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F650">
+      <c r="F650" s="72">
         <v>62850</v>
       </c>
       <c r="G650" t="s">
@@ -25909,7 +25973,7 @@
       <c r="E651" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F651">
+      <c r="F651" s="72">
         <v>9189</v>
       </c>
       <c r="G651" t="s">
@@ -25935,7 +25999,7 @@
       <c r="E652" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F652">
+      <c r="F652" s="72">
         <v>9189</v>
       </c>
       <c r="G652" t="s">
@@ -25961,7 +26025,7 @@
       <c r="E653" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F653">
+      <c r="F653" s="72">
         <v>9398</v>
       </c>
       <c r="G653" t="s">
@@ -25987,7 +26051,7 @@
       <c r="E654" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F654">
+      <c r="F654" s="72">
         <v>9396</v>
       </c>
       <c r="G654" t="s">
@@ -26013,7 +26077,7 @@
       <c r="E655" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F655">
+      <c r="F655" s="72">
         <v>9393</v>
       </c>
       <c r="G655" t="s">
@@ -26039,7 +26103,7 @@
       <c r="E656" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F656">
+      <c r="F656" s="72">
         <v>7296</v>
       </c>
       <c r="G656" t="s">
@@ -26065,7 +26129,7 @@
       <c r="E657" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F657">
+      <c r="F657" s="72">
         <v>6786</v>
       </c>
       <c r="G657" t="s">
@@ -26091,7 +26155,7 @@
       <c r="E658" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F658">
+      <c r="F658" s="72">
         <v>8040</v>
       </c>
       <c r="G658" t="s">
@@ -26117,7 +26181,7 @@
       <c r="E659" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F659">
+      <c r="F659" s="72">
         <v>9616</v>
       </c>
       <c r="G659" t="s">
@@ -26143,7 +26207,7 @@
       <c r="E660" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="F660">
+      <c r="F660" s="72">
         <v>10842</v>
       </c>
       <c r="G660" t="s">
@@ -26154,10 +26218,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I660" xr:uid="{0F6A7D78-92EA-47A0-BC0F-20805E66886E}"/>
+  <autoFilter ref="A1:I660" xr:uid="{0F6A7D78-92EA-47A0-BC0F-20805E66886E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:I242">
+      <sortCondition sortBy="cellColor" ref="C1:C660" dxfId="1"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E1:E13 E243:E660" numberStoredAsText="1"/>
+  </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>